<commit_message>
Update benchmark data in XLSX file
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="191">
   <si>
     <t>Model</t>
   </si>
@@ -53,6 +53,24 @@
     <t>Date</t>
   </si>
   <si>
+    <t>UI-TARS-1.5 (100 steps)</t>
+  </si>
+  <si>
+    <t>ByteDance Seed &amp; Tsinghua University</t>
+  </si>
+  <si>
+    <t>https://seed-tars.com/1.5</t>
+  </si>
+  <si>
+    <t>Qin et al., '24</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Apr 17, 2025</t>
+  </si>
+  <si>
     <t>OpenAI CUA (200 steps)</t>
   </si>
   <si>
@@ -65,9 +83,6 @@
     <t>OpenAI, '24</t>
   </si>
   <si>
-    <t>—</t>
-  </si>
-  <si>
     <t>Jan 24, 2025</t>
   </si>
   <si>
@@ -116,13 +131,7 @@
     <t>UI-TARS-72B-DPO (50 steps)</t>
   </si>
   <si>
-    <t>ByteDance Seed &amp; Tsinghua University</t>
-  </si>
-  <si>
     <t>https://github.com/bytedance/UI-TARS</t>
-  </si>
-  <si>
-    <t>Qin et al., '24</t>
   </si>
   <si>
     <t>Jan 21, 2025</t>
@@ -1538,10 +1547,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1576,14 +1585,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -1593,12 +1602,11 @@
         <v>11</v>
       </c>
       <c r="F2">
-        <v>38.1</v>
+        <v>42.5</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1617,7 +1625,7 @@
         <v>11</v>
       </c>
       <c r="F3">
-        <v>34.5</v>
+        <v>38.1</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
@@ -1640,41 +1648,41 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>34.5</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -1688,35 +1696,35 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
-        <v>26</v>
+      <c r="F6">
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7">
-        <v>24.6</v>
+      <c r="F7" t="s">
+        <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -1725,670 +1733,670 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8">
-        <v>22.7</v>
+        <v>24.6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9">
-        <v>22</v>
+        <v>22.7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>38</v>
+      <c r="F10">
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11">
-        <v>19.7</v>
+      <c r="F11" t="s">
+        <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" t="s">
-        <v>41</v>
+      <c r="F12">
+        <v>19.7</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13">
-        <v>18.8</v>
+      <c r="F13" t="s">
+        <v>44</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15">
-        <v>17.7</v>
+        <v>18.7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16">
-        <v>17.04</v>
+        <v>17.7</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" t="s">
-        <v>51</v>
+      <c r="F17">
+        <v>17.04</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F18">
-        <v>15.15</v>
+      <c r="F18" t="s">
+        <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19">
-        <v>14.9</v>
+        <v>15.15</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20">
-        <v>14.79</v>
+        <v>14.9</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="F21">
-        <v>14.63</v>
+        <v>14.79</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
       </c>
       <c r="F22">
-        <v>11.65</v>
+        <v>14.63</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
         <v>65</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" t="s">
-        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
       </c>
       <c r="F23">
-        <v>10.26</v>
+        <v>11.65</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
       </c>
       <c r="F24">
+        <v>10.26</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25">
         <v>9.21</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25">
-        <v>8.8</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
         <v>76</v>
       </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26">
+        <v>8.8</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26">
-        <v>8.7</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
         <v>81</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>82</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" t="s">
-        <v>84</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
       </c>
       <c r="F27">
-        <v>8.22</v>
+        <v>8.7</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>87</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>8.22</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D28" t="s">
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
         <v>89</v>
       </c>
-      <c r="E28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28">
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29">
         <v>8.12</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="G29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
         <v>93</v>
       </c>
-      <c r="E29" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29">
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30">
         <v>7.81</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="G30" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E30" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31">
         <v>7.69</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="G31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D31" t="s">
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>102</v>
       </c>
-      <c r="E31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31">
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32">
         <v>5.8</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32">
-        <v>5.4</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" t="s">
         <v>100</v>
       </c>
-      <c r="C33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" t="s">
-        <v>108</v>
-      </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F33">
         <v>5.4</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F34">
-        <v>5.26</v>
+        <v>5.4</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F35">
-        <v>5.03</v>
+        <v>5.26</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -2397,19 +2405,19 @@
         <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
         <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F36">
-        <v>3.77</v>
+        <v>5.03</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>115</v>
@@ -2421,46 +2429,46 @@
         <v>116</v>
       </c>
       <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
         <v>117</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37">
+        <v>3.77</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37">
-        <v>3.33</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" t="s">
         <v>120</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>121</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>122</v>
       </c>
-      <c r="D38" t="s">
-        <v>35</v>
-      </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F38">
-        <v>2.42</v>
+        <v>3.33</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="H38" s="3"/>
     </row>
@@ -2475,25 +2483,25 @@
         <v>125</v>
       </c>
       <c r="D39" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F39">
         <v>2.42</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" t="s">
         <v>127</v>
-      </c>
-      <c r="B40" t="s">
-        <v>71</v>
       </c>
       <c r="C40" t="s">
         <v>128</v>
@@ -2502,65 +2510,90 @@
         <v>129</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F40">
         <v>2.42</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
         <v>130</v>
       </c>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
         <v>131</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>132</v>
       </c>
-      <c r="C41" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41">
+        <v>2.42</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E41" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41">
-        <v>1.88</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>134</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D42" t="s">
         <v>136</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F42">
+        <v>1.88</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>137</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43">
         <v>1.11</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>103</v>
+      <c r="G43" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C28" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://seed-tars.com/1.5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2606,39 +2639,39 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F2">
         <v>22.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -2647,306 +2680,306 @@
         <v>16.6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F4">
         <v>12.24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F5">
         <v>11.36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F6">
         <v>10.82</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F7">
         <v>10.3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F8">
         <v>6.87</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F9">
         <v>6.21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F10">
         <v>4.81</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>4.32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F12">
         <v>2.98</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F13">
         <v>2.7</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F14">
         <v>2.69</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F15">
         <v>2.37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F16">
         <v>1.61</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2994,16 +3027,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -3012,67 +3045,67 @@
         <v>23.85</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F3">
         <v>20.58</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F4">
         <v>20.48</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -3081,21 +3114,21 @@
         <v>19.39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -3104,21 +3137,21 @@
         <v>17.34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -3127,283 +3160,283 @@
         <v>13.55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F8">
         <v>12.17</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F9">
         <v>11.21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F10">
         <v>11.11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>9.04</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F12">
         <v>8.94</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F13">
         <v>6.21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F14">
         <v>5.1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F15">
         <v>4.41</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F16">
         <v>3.5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F17">
         <v>3.48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F18">
         <v>2.42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F19">
         <v>1.32</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3451,16 +3484,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -3469,237 +3502,237 @@
         <v>24.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F3">
         <v>11.77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F4">
         <v>8.4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F5">
         <v>7.79</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F6">
         <v>6.72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F7">
         <v>5.4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F8">
         <v>4.59</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F9">
         <v>3.5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F10">
         <v>2.42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>1.06</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F12">
         <v>0.99</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark data in XLSX file with latest changes
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13100"/>
+    <workbookView windowWidth="27660" windowHeight="13120"/>
   </bookViews>
   <sheets>
     <sheet name="Screenshot" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="197">
   <si>
     <t>Model</t>
   </si>
@@ -65,24 +65,27 @@
     <t>Seed-TARS, '25</t>
   </si>
   <si>
+    <t>Active parameter &gt;20B?</t>
+  </si>
+  <si>
+    <t>Apr 17, 2025</t>
+  </si>
+  <si>
+    <t>Agent S2 w/ Gemini 2.5 (50 steps)</t>
+  </si>
+  <si>
+    <t>Simular Research</t>
+  </si>
+  <si>
+    <t>https://github.com/simular-ai/Agent-S</t>
+  </si>
+  <si>
+    <t>Simular Research, '25</t>
+  </si>
+  <si>
     <t>—</t>
   </si>
   <si>
-    <t>Apr 17, 2025</t>
-  </si>
-  <si>
-    <t>Agent S2 w/ Gemini 2.5 (50 steps)</t>
-  </si>
-  <si>
-    <t>Simular Research</t>
-  </si>
-  <si>
-    <t>https://github.com/simular-ai/Agent-S</t>
-  </si>
-  <si>
-    <t>Simular Research, '25</t>
-  </si>
-  <si>
     <t>Apr 18, 2025</t>
   </si>
   <si>
@@ -129,6 +132,9 @@
   </si>
   <si>
     <t>Simular Agent S2 (15 steps)</t>
+  </si>
+  <si>
+    <t>UI-TARS-1.5 7B (100 steps)</t>
   </si>
   <si>
     <t>Claude 3.7 Sonnet (50 steps)</t>
@@ -1552,10 +1558,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1627,133 +1633,133 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>41.4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>38.1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>34.5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>26.92</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H8" s="3"/>
     </row>
@@ -1762,94 +1768,94 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>24.6</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F10">
-        <v>22.7</v>
+        <v>24.6</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>22.7</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>22</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
       <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -1858,46 +1864,46 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>19.7</v>
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>48</v>
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>19.7</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -1906,118 +1912,118 @@
         <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>18.8</v>
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F16">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F17">
-        <v>17.7</v>
+        <v>18.7</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F18">
-        <v>17.04</v>
+        <v>17.7</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
       <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>17.04</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H19" s="3"/>
     </row>
@@ -2026,604 +2032,629 @@
         <v>59</v>
       </c>
       <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>15.15</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F21">
-        <v>14.9</v>
+        <v>15.15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F22">
-        <v>14.79</v>
+        <v>14.9</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F23">
-        <v>14.63</v>
+        <v>14.79</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" t="s">
-        <v>69</v>
-      </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F24">
-        <v>11.65</v>
+        <v>14.63</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <v>11.65</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25">
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26">
         <v>10.26</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="G26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
         <v>75</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B27" t="s">
         <v>76</v>
       </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26">
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27">
         <v>9.21</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27">
-        <v>8.8</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28">
+        <v>8.8</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28">
-        <v>8.7</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
         <v>88</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>8.7</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29">
-        <v>8.22</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
         <v>93</v>
       </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>8.22</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C30" t="s">
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
         <v>95</v>
       </c>
-      <c r="D30" t="s">
+      <c r="B31" t="s">
         <v>96</v>
       </c>
-      <c r="E30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30">
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31">
         <v>8.12</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="G31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>99</v>
       </c>
-      <c r="D31" t="s">
+      <c r="B32" t="s">
         <v>100</v>
       </c>
-      <c r="E31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31">
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32">
         <v>7.81</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="G32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D32" t="s">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
-      <c r="E32" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33">
         <v>7.69</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="G33" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C33" t="s">
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
         <v>108</v>
       </c>
-      <c r="D33" t="s">
+      <c r="B34" t="s">
         <v>109</v>
       </c>
-      <c r="E33" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33">
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34">
         <v>5.8</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34">
-        <v>5.4</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F35">
         <v>5.4</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F36">
-        <v>5.26</v>
+        <v>5.4</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F37">
-        <v>5.03</v>
+        <v>5.26</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
         <v>120</v>
       </c>
-      <c r="B38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38">
+        <v>5.03</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" t="s">
-        <v>81</v>
-      </c>
-      <c r="F38">
-        <v>3.77</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
         <v>123</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39">
+        <v>3.77</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C39" t="s">
-        <v>125</v>
-      </c>
-      <c r="D39" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39">
-        <v>3.33</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" t="s">
         <v>127</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>128</v>
       </c>
-      <c r="C40" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" t="s">
-        <v>42</v>
-      </c>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F40">
-        <v>2.42</v>
+        <v>3.33</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" t="s">
         <v>130</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>131</v>
       </c>
-      <c r="C41" t="s">
-        <v>132</v>
-      </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F41">
         <v>2.42</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" t="s">
         <v>134</v>
       </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>135</v>
       </c>
-      <c r="D42" t="s">
-        <v>136</v>
-      </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F42">
         <v>2.42</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
         <v>137</v>
       </c>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
+      <c r="D43" t="s">
         <v>138</v>
       </c>
-      <c r="B43" t="s">
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43">
+        <v>2.42</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" t="s">
-        <v>140</v>
-      </c>
-      <c r="E43" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43">
-        <v>1.88</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
         <v>141</v>
       </c>
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
       <c r="C44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" t="s">
         <v>142</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44">
+        <v>1.88</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
         <v>143</v>
       </c>
-      <c r="E44" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44">
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45">
         <v>1.11</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>110</v>
+      <c r="G45" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C29" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C30" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
     <hyperlink ref="C2" r:id="rId2" display="https://seed-tars.com/1.5"/>
     <hyperlink ref="C3" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
+    <hyperlink ref="C8" r:id="rId2" display="https://seed-tars.com/1.5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2669,347 +2700,347 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F2">
         <v>22.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>16.6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F4">
         <v>12.24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F5">
         <v>11.36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F6">
         <v>10.82</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F7">
         <v>10.3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F8">
         <v>6.87</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F9">
         <v>6.21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F10">
         <v>4.81</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F11">
         <v>4.32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12">
         <v>2.98</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F13">
         <v>2.7</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F14">
         <v>2.69</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F15">
         <v>2.37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F16">
         <v>1.61</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3057,416 +3088,416 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>23.85</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F3">
         <v>20.58</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F4">
         <v>20.48</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>19.39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>17.34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>13.55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F8">
         <v>12.17</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F9">
         <v>11.21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F10">
         <v>11.11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F11">
         <v>9.04</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12">
         <v>8.94</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F13">
         <v>6.21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F14">
         <v>5.1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F15">
         <v>4.41</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F16">
         <v>3.5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F17">
         <v>3.48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F18">
         <v>2.42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F19">
         <v>1.32</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3514,255 +3545,255 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>24.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F3">
         <v>11.77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F4">
         <v>8.4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F5">
         <v>7.79</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F6">
         <v>6.72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F7">
         <v>5.4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F8">
         <v>4.59</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F9">
         <v>3.5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F10">
         <v>2.42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F11">
         <v>1.06</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12">
         <v>0.99</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update trajectory link image in index.html and add new hello-click-here.gif; update benchmark data in XLSX file
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -47,7 +47,7 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Trajectories</t>
+    <t>TrajectoryLink</t>
   </si>
   <si>
     <t>Score</t>
@@ -1691,8 +1691,8 @@
   <sheetPr/>
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2948,7 +2948,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3399,7 +3399,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3924,7 +3924,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with latest performance metrics and trends for improved analysis.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13120" activeTab="3"/>
+    <workbookView windowWidth="27660" windowHeight="13120"/>
   </bookViews>
   <sheets>
     <sheet name="Screenshot" sheetId="1" r:id="rId1"/>
@@ -92,6 +92,9 @@
     <t>—</t>
   </si>
   <si>
+    <t>https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link</t>
+  </si>
+  <si>
     <t>Apr 18, 2025</t>
   </si>
   <si>
@@ -114,9 +117,6 @@
   </si>
   <si>
     <t>https://www.simular.ai/agent-s</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link</t>
   </si>
   <si>
     <t>Mar 13, 2025</t>
@@ -1691,8 +1691,8 @@
   <sheetPr/>
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1773,29 +1773,29 @@
       <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
-        <v>19</v>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="G3">
         <v>41.4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1807,19 +1807,19 @@
         <v>38.1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -1827,8 +1827,8 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="G5">
         <v>34.5</v>
@@ -1873,7 +1873,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -1881,8 +1881,8 @@
       <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
-        <v>19</v>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G7">
         <v>27</v>
@@ -2059,13 +2059,13 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
@@ -2077,7 +2077,7 @@
         <v>19.7</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I14" s="5"/>
     </row>
@@ -2572,7 +2572,7 @@
         <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
         <v>110</v>
@@ -2626,7 +2626,7 @@
         <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
         <v>110</v>
@@ -2680,7 +2680,7 @@
         <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
         <v>110</v>
@@ -2707,13 +2707,13 @@
         <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
         <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E38" t="s">
         <v>87</v>
@@ -2734,13 +2734,13 @@
         <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
         <v>133</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E39" t="s">
         <v>87</v>
@@ -2926,7 +2926,7 @@
     <hyperlink ref="F10" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
     <hyperlink ref="F32" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
     <hyperlink ref="F36" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
-    <hyperlink ref="F5" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
     <hyperlink ref="F35" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
     <hyperlink ref="F43" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
     <hyperlink ref="F34" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
@@ -2936,6 +2936,8 @@
     <hyperlink ref="F40" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
     <hyperlink ref="F42" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
     <hyperlink ref="F44" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
+    <hyperlink ref="F3" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F7" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3039,7 +3041,7 @@
         <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>173</v>
@@ -3065,13 +3067,13 @@
         <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>87</v>
@@ -3091,7 +3093,7 @@
         <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>110</v>
@@ -3169,13 +3171,13 @@
         <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
@@ -3299,7 +3301,7 @@
         <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>192</v>
@@ -3467,7 +3469,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>207</v>
@@ -3493,7 +3495,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>207</v>
@@ -3594,7 +3596,7 @@
         <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>110</v>
@@ -3620,13 +3622,13 @@
         <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
@@ -3672,7 +3674,7 @@
         <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>110</v>
@@ -3724,13 +3726,13 @@
         <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
         <v>87</v>
@@ -3923,8 +3925,8 @@
   <sheetPr/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3989,7 +3991,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>110</v>
@@ -4015,7 +4017,7 @@
         <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>110</v>
@@ -4119,13 +4121,13 @@
         <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>129</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>87</v>
@@ -4145,13 +4147,13 @@
         <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with new performance metrics for enhanced analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13120"/>
+    <workbookView windowWidth="27660" windowHeight="13260"/>
   </bookViews>
   <sheets>
     <sheet name="Screenshot" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="247">
   <si>
     <t>Model</t>
   </si>
@@ -107,319 +107,340 @@
     <t>https://openai.com/index/computer-using-agent/</t>
   </si>
   <si>
+    <t>OpenAI, '25</t>
+  </si>
+  <si>
+    <t>Jan 24, 2025</t>
+  </si>
+  <si>
+    <t>InfantAgent (50 steps)</t>
+  </si>
+  <si>
+    <t>Evolution intelligence &amp; University of Minnesota</t>
+  </si>
+  <si>
+    <t>https://github.com/bin123apple/InfantAgent</t>
+  </si>
+  <si>
+    <t>Planner: Claude-3.7 Sonnet，Grounder: UI-TARS-1.5-7B</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Apr 30, 2025</t>
+  </si>
+  <si>
+    <t>Agent S2 w/ Claude 3.7 (50 steps)</t>
+  </si>
+  <si>
+    <t>https://www.simular.ai/agent-s</t>
+  </si>
+  <si>
+    <t>Mar 13, 2025</t>
+  </si>
+  <si>
+    <t>Claude 3.7 Sonnet (100 steps)</t>
+  </si>
+  <si>
+    <t>Anthropic</t>
+  </si>
+  <si>
+    <t>https://www.anthropic.com/research/visible-extended-thinking</t>
+  </si>
+  <si>
+    <t>Anthropic, '25</t>
+  </si>
+  <si>
+    <t>~ 28</t>
+  </si>
+  <si>
+    <t>Feb 24, 2025</t>
+  </si>
+  <si>
+    <t>Simular Agent S2 (15 steps)</t>
+  </si>
+  <si>
+    <t>UI-TARS-1.5 7B (100 steps)</t>
+  </si>
+  <si>
+    <t>Claude 3.7 Sonnet (50 steps)</t>
+  </si>
+  <si>
+    <t>~ 26</t>
+  </si>
+  <si>
+    <t>UI-TARS-72B-DPO (50 steps)</t>
+  </si>
+  <si>
+    <t>https://github.com/bytedance/UI-TARS</t>
+  </si>
+  <si>
+    <t>Qin et al., '24</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Jan 21, 2025</t>
+  </si>
+  <si>
+    <t>UI-TARS-72B-DPO (15 steps)</t>
+  </si>
+  <si>
+    <t>Claude 3.5 Sonnet (50 steps)</t>
+  </si>
+  <si>
+    <t>https://assets.anthropic.com/m/1cd9d098ac3e6467/original/Claude-3-Model-Card-October-Addendum.pdf</t>
+  </si>
+  <si>
+    <t>Anthropic, '24</t>
+  </si>
+  <si>
+    <t>Oct 22, 2024</t>
+  </si>
+  <si>
+    <t>Claude 3.5 Sonnet (new) (100 steps)</t>
+  </si>
+  <si>
+    <t>~ 21</t>
+  </si>
+  <si>
+    <t>OpenAI CUA (15 steps)</t>
+  </si>
+  <si>
+    <t>Claude 3.5 Sonnet (new) (50 steps)</t>
+  </si>
+  <si>
+    <t>~ 19.5</t>
+  </si>
+  <si>
+    <t>UI-TARS-72B-SFT (15 steps)</t>
+  </si>
+  <si>
+    <t>UI-TARS-7B-DPO (15 steps)</t>
+  </si>
+  <si>
+    <t>UI-TARS-7B-SFT (15 steps)</t>
+  </si>
+  <si>
+    <t>Aguvis-72B w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>Salesforce &amp; The University of Hong Kong</t>
+  </si>
+  <si>
+    <t>https://aguvis-project.github.io/</t>
+  </si>
+  <si>
+    <t>Xu et al., '24</t>
+  </si>
+  <si>
+    <t>Nov 22, 2024</t>
+  </si>
+  <si>
+    <t>Claude 3.7 Sonnet (15 steps)</t>
+  </si>
+  <si>
+    <t>~ 15.5</t>
+  </si>
+  <si>
+    <t>Aria-UI w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>University of Hong Kong &amp; Rhymes AI</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2412.16256</t>
+  </si>
+  <si>
+    <t>Yang et al., '24</t>
+  </si>
+  <si>
+    <t>Dec 24, 2024</t>
+  </si>
+  <si>
+    <t>Claude 3.5 Sonnet (15 steps)</t>
+  </si>
+  <si>
+    <t>Aguvis-7B w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>OS-Atlas-Base-7B w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>Shanghai AI Lab</t>
+  </si>
+  <si>
+    <t>https://osatlas.github.io/</t>
+  </si>
+  <si>
+    <t>Wu et al., '24</t>
+  </si>
+  <si>
+    <t>Oct 30, 2024</t>
+  </si>
+  <si>
+    <t>OS-Atlas-Base-4B w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>Aguvis-72B</t>
+  </si>
+  <si>
+    <t>SeeClick w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>Nanjing University &amp; Shanghai AI Lab</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2401.10935</t>
+  </si>
+  <si>
+    <t>Cheng et al., '24</t>
+  </si>
+  <si>
+    <t>Qwen2.5-vl-72B</t>
+  </si>
+  <si>
+    <t>Alibaba Cloud, Qwen Team</t>
+  </si>
+  <si>
+    <t>https://qwenlm.github.io/blog/qwen2.5-vl/</t>
+  </si>
+  <si>
+    <t>Qwen Team, '25</t>
+  </si>
+  <si>
+    <t>t=1.0, top-p=0.9</t>
+  </si>
+  <si>
+    <t>Jan 26, 2025</t>
+  </si>
+  <si>
+    <t>Ponder&amp;Press w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>Shenzhen International Graduate School, Tsinghua University</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2412.01268</t>
+  </si>
+  <si>
+    <t>Wang et al., '24</t>
+  </si>
+  <si>
+    <t>Dec 2, 2024</t>
+  </si>
+  <si>
+    <t>Kimi-VL</t>
+  </si>
+  <si>
+    <t>Kimi &amp; The University of Hong Kong</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2504.07491</t>
+  </si>
+  <si>
+    <t>Kimi Team, '25</t>
+  </si>
+  <si>
+    <t>April 10, 2025</t>
+  </si>
+  <si>
+    <t>CogAgent-9B-20241220</t>
+  </si>
+  <si>
+    <t>Tsinghua University &amp; Zhipu AI</t>
+  </si>
+  <si>
+    <t>https://cogagent.aminer.cn/blog#/articles/cogagent-9b-20241220-technical-report-en</t>
+  </si>
+  <si>
+    <t>Hong et al., '24</t>
+  </si>
+  <si>
+    <t>CRADLE w/ GPT-4o</t>
+  </si>
+  <si>
+    <t>BAAI</t>
+  </si>
+  <si>
+    <t>https://baai-agents.github.io/Cradle/</t>
+  </si>
+  <si>
+    <t>BAAI, '24</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Jun 14, 2024</t>
+  </si>
+  <si>
+    <t>GPT-4 Vision</t>
+  </si>
+  <si>
+    <t>https://openai.com/research/gpt-4v-system-card</t>
+  </si>
+  <si>
+    <t>OpenAI, '23</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>May 24, 2024</t>
+  </si>
+  <si>
+    <t>Gemini-Pro Vision</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2312.11805</t>
+  </si>
+  <si>
+    <t>Gemini Team, Google, '23</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Mar 20, 2024</t>
+  </si>
+  <si>
+    <t>GPT-4 Vision (0409)</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link</t>
+  </si>
+  <si>
+    <t>April 23, 2024</t>
+  </si>
+  <si>
+    <t>Gemini-Pro-1.5</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2403.05530</t>
+  </si>
+  <si>
+    <t>Gemini Team, Google, '24</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link</t>
+  </si>
+  <si>
+    <t>May 3, 2024</t>
+  </si>
+  <si>
+    <t>GPT-4o</t>
+  </si>
+  <si>
+    <t>https://openai.com/index/hello-gpt-4o/</t>
+  </si>
+  <si>
     <t>OpenAI, '24</t>
-  </si>
-  <si>
-    <t>Jan 24, 2025</t>
-  </si>
-  <si>
-    <t>Agent S2 w/ Claude 3.7 (50 steps)</t>
-  </si>
-  <si>
-    <t>https://www.simular.ai/agent-s</t>
-  </si>
-  <si>
-    <t>Mar 13, 2025</t>
-  </si>
-  <si>
-    <t>Claude 3.7 Sonnet (100 steps)</t>
-  </si>
-  <si>
-    <t>Anthropic</t>
-  </si>
-  <si>
-    <t>https://www.anthropic.com/research/visible-extended-thinking</t>
-  </si>
-  <si>
-    <t>Anthropic, '25</t>
-  </si>
-  <si>
-    <t>~ 28</t>
-  </si>
-  <si>
-    <t>Feb 24, 2025</t>
-  </si>
-  <si>
-    <t>Simular Agent S2 (15 steps)</t>
-  </si>
-  <si>
-    <t>UI-TARS-1.5 7B (100 steps)</t>
-  </si>
-  <si>
-    <t>Claude 3.7 Sonnet (50 steps)</t>
-  </si>
-  <si>
-    <t>~ 26</t>
-  </si>
-  <si>
-    <t>UI-TARS-72B-DPO (50 steps)</t>
-  </si>
-  <si>
-    <t>https://github.com/bytedance/UI-TARS</t>
-  </si>
-  <si>
-    <t>Qin et al., '24</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>Jan 21, 2025</t>
-  </si>
-  <si>
-    <t>UI-TARS-72B-DPO (15 steps)</t>
-  </si>
-  <si>
-    <t>Claude 3.5 Sonnet (50 steps)</t>
-  </si>
-  <si>
-    <t>https://assets.anthropic.com/m/1cd9d098ac3e6467/original/Claude-3-Model-Card-October-Addendum.pdf</t>
-  </si>
-  <si>
-    <t>Anthropic, '24</t>
-  </si>
-  <si>
-    <t>Oct 22, 2024</t>
-  </si>
-  <si>
-    <t>Claude 3.5 Sonnet (new) (100 steps)</t>
-  </si>
-  <si>
-    <t>~ 21</t>
-  </si>
-  <si>
-    <t>OpenAI CUA (15 steps)</t>
-  </si>
-  <si>
-    <t>Claude 3.5 Sonnet (new) (50 steps)</t>
-  </si>
-  <si>
-    <t>~ 19.5</t>
-  </si>
-  <si>
-    <t>UI-TARS-72B-SFT (15 steps)</t>
-  </si>
-  <si>
-    <t>UI-TARS-7B-DPO (15 steps)</t>
-  </si>
-  <si>
-    <t>UI-TARS-7B-SFT (15 steps)</t>
-  </si>
-  <si>
-    <t>Aguvis-72B w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Salesforce &amp; The University of Hong Kong</t>
-  </si>
-  <si>
-    <t>https://aguvis-project.github.io/</t>
-  </si>
-  <si>
-    <t>Xu et al., '24</t>
-  </si>
-  <si>
-    <t>Nov 22, 2024</t>
-  </si>
-  <si>
-    <t>Claude 3.7 Sonnet (15 steps)</t>
-  </si>
-  <si>
-    <t>~ 15.5</t>
-  </si>
-  <si>
-    <t>Aria-UI w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>University of Hong Kong &amp; Rhymes AI</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2412.16256</t>
-  </si>
-  <si>
-    <t>Yang et al., '24</t>
-  </si>
-  <si>
-    <t>Dec 24, 2024</t>
-  </si>
-  <si>
-    <t>Claude 3.5 Sonnet (15 steps)</t>
-  </si>
-  <si>
-    <t>Aguvis-7B w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>OS-Atlas-Base-7B w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Shanghai AI Lab</t>
-  </si>
-  <si>
-    <t>https://osatlas.github.io/</t>
-  </si>
-  <si>
-    <t>Wu et al., '24</t>
-  </si>
-  <si>
-    <t>Oct 30, 2024</t>
-  </si>
-  <si>
-    <t>OS-Atlas-Base-4B w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Aguvis-72B</t>
-  </si>
-  <si>
-    <t>SeeClick w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Nanjing University &amp; Shanghai AI Lab</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2401.10935</t>
-  </si>
-  <si>
-    <t>Cheng et al., '24</t>
-  </si>
-  <si>
-    <t>Qwen2.5-vl-72B</t>
-  </si>
-  <si>
-    <t>Alibaba Cloud, Qwen Team</t>
-  </si>
-  <si>
-    <t>https://qwenlm.github.io/blog/qwen2.5-vl/</t>
-  </si>
-  <si>
-    <t>Qwen Team, '25</t>
-  </si>
-  <si>
-    <t>t=1.0, top-p=0.9</t>
-  </si>
-  <si>
-    <t>Jan 26, 2025</t>
-  </si>
-  <si>
-    <t>Ponder&amp;Press w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Shenzhen International Graduate School, Tsinghua University</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2412.01268</t>
-  </si>
-  <si>
-    <t>Wang et al., '24</t>
-  </si>
-  <si>
-    <t>Dec 2, 2024</t>
-  </si>
-  <si>
-    <t>Kimi-VL</t>
-  </si>
-  <si>
-    <t>Kimi &amp; The University of Hong Kong</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2504.07491</t>
-  </si>
-  <si>
-    <t>Kimi Team, '25</t>
-  </si>
-  <si>
-    <t>April 10, 2025</t>
-  </si>
-  <si>
-    <t>CogAgent-9B-20241220</t>
-  </si>
-  <si>
-    <t>Tsinghua University &amp; Zhipu AI</t>
-  </si>
-  <si>
-    <t>https://cogagent.aminer.cn/blog#/articles/cogagent-9b-20241220-technical-report-en</t>
-  </si>
-  <si>
-    <t>Hong et al., '24</t>
-  </si>
-  <si>
-    <t>CRADLE w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>BAAI</t>
-  </si>
-  <si>
-    <t>https://baai-agents.github.io/Cradle/</t>
-  </si>
-  <si>
-    <t>BAAI, '24</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link</t>
-  </si>
-  <si>
-    <t>Jun 14, 2024</t>
-  </si>
-  <si>
-    <t>GPT-4 Vision</t>
-  </si>
-  <si>
-    <t>https://openai.com/research/gpt-4v-system-card</t>
-  </si>
-  <si>
-    <t>OpenAI, '23</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>May 24, 2024</t>
-  </si>
-  <si>
-    <t>Gemini-Pro Vision</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2312.11805</t>
-  </si>
-  <si>
-    <t>Gemini Team, Google, '23</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link</t>
-  </si>
-  <si>
-    <t>Mar 20, 2024</t>
-  </si>
-  <si>
-    <t>GPT-4 Vision (0409)</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link</t>
-  </si>
-  <si>
-    <t>April 23, 2024</t>
-  </si>
-  <si>
-    <t>Gemini-Pro-1.5</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2403.05530</t>
-  </si>
-  <si>
-    <t>Gemini Team, Google, '24</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link</t>
-  </si>
-  <si>
-    <t>May 3, 2024</t>
-  </si>
-  <si>
-    <t>GPT-4o</t>
-  </si>
-  <si>
-    <t>https://openai.com/index/hello-gpt-4o/</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link</t>
@@ -1363,12 +1384,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1689,10 +1711,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1782,7 +1804,7 @@
       <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -1809,128 +1831,125 @@
       <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="G5">
-        <v>34.5</v>
+        <v>35.27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>34.5</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>27</v>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G8">
-        <v>26.92</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -1938,74 +1957,74 @@
       <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
-        <v>39</v>
+      <c r="G9">
+        <v>26.92</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10">
-        <v>24.6</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
-        <v>19</v>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="G11">
-        <v>22.7</v>
+        <v>24.6</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
@@ -2020,25 +2039,25 @@
         <v>19</v>
       </c>
       <c r="G12">
-        <v>22</v>
+        <v>22.7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -2046,26 +2065,26 @@
       <c r="F13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" t="s">
-        <v>51</v>
+      <c r="G13">
+        <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
@@ -2073,26 +2092,26 @@
       <c r="F14" t="s">
         <v>19</v>
       </c>
-      <c r="G14">
-        <v>19.7</v>
+      <c r="G14" t="s">
+        <v>57</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -2100,53 +2119,53 @@
       <c r="F15" t="s">
         <v>19</v>
       </c>
-      <c r="G15" t="s">
-        <v>54</v>
+      <c r="G15">
+        <v>19.7</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16">
-        <v>18.8</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -2155,25 +2174,25 @@
         <v>19</v>
       </c>
       <c r="G17">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -2182,25 +2201,25 @@
         <v>19</v>
       </c>
       <c r="G18">
-        <v>17.7</v>
+        <v>18.7</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -2209,25 +2228,25 @@
         <v>19</v>
       </c>
       <c r="G19">
-        <v>17.04</v>
+        <v>17.7</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -2235,26 +2254,26 @@
       <c r="F20" t="s">
         <v>19</v>
       </c>
-      <c r="G20" t="s">
-        <v>64</v>
+      <c r="G20">
+        <v>17.04</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -2262,26 +2281,26 @@
       <c r="F21" t="s">
         <v>19</v>
       </c>
-      <c r="G21">
-        <v>15.15</v>
+      <c r="G21" t="s">
+        <v>70</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -2290,25 +2309,25 @@
         <v>19</v>
       </c>
       <c r="G22">
-        <v>14.9</v>
+        <v>15.15</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
@@ -2317,25 +2336,25 @@
         <v>19</v>
       </c>
       <c r="G23">
-        <v>14.79</v>
+        <v>14.9</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -2344,25 +2363,25 @@
         <v>19</v>
       </c>
       <c r="G24">
-        <v>14.63</v>
+        <v>14.79</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I24" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -2371,25 +2390,25 @@
         <v>19</v>
       </c>
       <c r="G25">
-        <v>11.65</v>
+        <v>14.63</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2398,66 +2417,66 @@
         <v>19</v>
       </c>
       <c r="G26">
+        <v>11.65</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27">
         <v>10.26</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="H27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28">
+        <v>9.21</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27">
-        <v>9.21</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28">
-        <v>8.8</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I28" s="5"/>
+      <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
@@ -2473,31 +2492,31 @@
         <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="F29" t="s">
         <v>19</v>
       </c>
       <c r="G29">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I29" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
@@ -2506,100 +2525,100 @@
         <v>19</v>
       </c>
       <c r="G30">
-        <v>8.22</v>
+        <v>8.7</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I30" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" t="s">
         <v>101</v>
       </c>
+      <c r="C31" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
       </c>
       <c r="G31">
+        <v>8.22</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32">
         <v>8.12</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B32" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32">
-        <v>7.81</v>
-      </c>
       <c r="H32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:9">
+        <v>75</v>
+      </c>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>109</v>
       </c>
       <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33">
+        <v>7.81</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
         <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G33">
-        <v>7.69</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" t="s">
-        <v>115</v>
       </c>
       <c r="C34" t="s">
         <v>116</v>
@@ -2608,336 +2627,365 @@
         <v>117</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>118</v>
       </c>
       <c r="G34">
-        <v>5.8</v>
+        <v>7.69</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G35">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I35" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>126</v>
+        <v>93</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="G36">
         <v>5.4</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I36" s="5"/>
+        <v>128</v>
+      </c>
+      <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
-      </c>
-      <c r="F37" t="s">
-        <v>19</v>
+        <v>93</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G37">
-        <v>5.26</v>
+        <v>5.4</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I37" s="5"/>
+        <v>133</v>
+      </c>
+      <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>130</v>
+        <v>93</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
       </c>
       <c r="G38">
-        <v>5.03</v>
+        <v>5.26</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I38" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G39">
-        <v>3.77</v>
+        <v>5.03</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I39" s="5"/>
+        <v>138</v>
+      </c>
+      <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" t="s">
         <v>136</v>
       </c>
-      <c r="B40" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" t="s">
-        <v>138</v>
-      </c>
-      <c r="D40" t="s">
-        <v>139</v>
-      </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G40">
-        <v>3.33</v>
+        <v>3.77</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I40" s="5"/>
+        <v>142</v>
+      </c>
+      <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41">
+        <v>3.33</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C41" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" t="s">
-        <v>87</v>
-      </c>
-      <c r="F41" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41">
-        <v>2.42</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I41" s="5"/>
+      <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>148</v>
+        <v>93</v>
+      </c>
+      <c r="F42" t="s">
+        <v>19</v>
       </c>
       <c r="G42">
         <v>2.42</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I42" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G43">
         <v>2.42</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:8">
+        <v>142</v>
+      </c>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E44" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G44">
-        <v>1.88</v>
+        <v>2.42</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>135</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D45" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E45" t="s">
-        <v>87</v>
-      </c>
-      <c r="F45" t="s">
-        <v>19</v>
+        <v>93</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="G45">
+        <v>1.88</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46">
         <v>1.11</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>119</v>
+      <c r="H46" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C30" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C31" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
     <hyperlink ref="C2" r:id="rId2" display="https://seed-tars.com/1.5"/>
     <hyperlink ref="C3" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C8" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
+    <hyperlink ref="C9" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
     <hyperlink ref="F2" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
-    <hyperlink ref="F10" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
-    <hyperlink ref="F32" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
-    <hyperlink ref="F36" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
-    <hyperlink ref="F5" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F35" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
-    <hyperlink ref="F43" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
-    <hyperlink ref="F34" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
-    <hyperlink ref="F33" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
-    <hyperlink ref="F39" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
-    <hyperlink ref="F38" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
-    <hyperlink ref="F40" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
-    <hyperlink ref="F42" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
-    <hyperlink ref="F44" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
+    <hyperlink ref="F11" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
+    <hyperlink ref="F33" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
+    <hyperlink ref="F37" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
+    <hyperlink ref="F6" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F36" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
+    <hyperlink ref="F44" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
+    <hyperlink ref="F35" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
+    <hyperlink ref="F34" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
+    <hyperlink ref="F40" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
+    <hyperlink ref="F39" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
+    <hyperlink ref="F41" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
+    <hyperlink ref="F43" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
+    <hyperlink ref="F45" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
     <hyperlink ref="F3" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F7" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="C5" r:id="rId18" display="https://github.com/bin123apple/InfantAgent"/>
+    <hyperlink ref="F5" r:id="rId19" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2986,19 +3034,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -3007,21 +3055,21 @@
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -3033,102 +3081,102 @@
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -3137,128 +3185,128 @@
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3267,111 +3315,111 @@
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3437,16 +3485,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -3458,24 +3506,24 @@
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3484,24 +3532,24 @@
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -3510,47 +3558,47 @@
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -3562,21 +3610,21 @@
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -3588,76 +3636,76 @@
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -3666,50 +3714,50 @@
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C12" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3718,76 +3766,76 @@
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -3796,102 +3844,102 @@
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -3900,7 +3948,7 @@
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3962,16 +4010,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -3983,76 +4031,76 @@
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -4061,50 +4109,50 @@
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -4113,128 +4161,128 @@
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -4243,7 +4291,7 @@
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with additional performance metrics for comprehensive analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="258">
   <si>
     <t>Model</t>
   </si>
@@ -158,6 +158,24 @@
     <t>Feb 24, 2025</t>
   </si>
   <si>
+    <t>Jedi-7B w/ GPT-4o (100 steps)</t>
+  </si>
+  <si>
+    <t>Salesforce &amp; The University of Hong Kong</t>
+  </si>
+  <si>
+    <t>https://osworld-grounding.github.io/</t>
+  </si>
+  <si>
+    <t>Xie et al., '25</t>
+  </si>
+  <si>
+    <t>avg 27.04, std 1.81</t>
+  </si>
+  <si>
+    <t>May 9, 2025</t>
+  </si>
+  <si>
     <t>Simular Agent S2 (15 steps)</t>
   </si>
   <si>
@@ -170,6 +188,12 @@
     <t>~ 26</t>
   </si>
   <si>
+    <t>Jedi-7B w/ GPT-4o (50 steps)</t>
+  </si>
+  <si>
+    <t>avg 25.02, std 1.30</t>
+  </si>
+  <si>
     <t>UI-TARS-72B-DPO (50 steps)</t>
   </si>
   <si>
@@ -185,6 +209,12 @@
     <t>Jan 21, 2025</t>
   </si>
   <si>
+    <t>Jedi-7B w/ GPT-4o (15 steps)</t>
+  </si>
+  <si>
+    <t>avg 22.74, std 0.51</t>
+  </si>
+  <si>
     <t>UI-TARS-72B-DPO (15 steps)</t>
   </si>
   <si>
@@ -200,6 +230,12 @@
     <t>Oct 22, 2024</t>
   </si>
   <si>
+    <t>Jedi-3B w/ GPT-4o (15 steps)</t>
+  </si>
+  <si>
+    <t>avg 21.8, std 0.19</t>
+  </si>
+  <si>
     <t>Claude 3.5 Sonnet (new) (100 steps)</t>
   </si>
   <si>
@@ -225,9 +261,6 @@
   </si>
   <si>
     <t>Aguvis-72B w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Salesforce &amp; The University of Hong Kong</t>
   </si>
   <si>
     <t>https://aguvis-project.github.io/</t>
@@ -1711,10 +1744,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1760,7 +1793,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
@@ -1786,7 +1819,7 @@
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
@@ -1840,13 +1873,13 @@
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="G5">
@@ -1916,67 +1949,67 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
       </c>
       <c r="G8">
-        <v>27</v>
+        <v>27.04</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
-        <v>19</v>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G9">
-        <v>26.92</v>
+        <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
@@ -1984,161 +2017,161 @@
       <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="G10" t="s">
-        <v>45</v>
+      <c r="G10">
+        <v>26.92</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11">
-        <v>24.6</v>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12">
+        <v>25.02</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12">
-        <v>22.7</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" t="s">
-        <v>19</v>
+      <c r="F13" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="G13">
-        <v>22</v>
+        <v>24.6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
       </c>
-      <c r="G14" t="s">
-        <v>57</v>
+      <c r="G14">
+        <v>22.74</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15">
+        <v>22.7</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15">
-        <v>19.7</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -2146,53 +2179,53 @@
       <c r="F16" t="s">
         <v>19</v>
       </c>
-      <c r="G16" t="s">
-        <v>60</v>
+      <c r="G16">
+        <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>21.8</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17">
-        <v>18.8</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -2200,26 +2233,26 @@
       <c r="F18" t="s">
         <v>19</v>
       </c>
-      <c r="G18">
-        <v>18.7</v>
+      <c r="G18" t="s">
+        <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -2228,25 +2261,25 @@
         <v>19</v>
       </c>
       <c r="G19">
-        <v>17.7</v>
+        <v>19.7</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -2254,26 +2287,26 @@
       <c r="F20" t="s">
         <v>19</v>
       </c>
-      <c r="G20">
-        <v>17.04</v>
+      <c r="G20" t="s">
+        <v>72</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -2281,26 +2314,26 @@
       <c r="F21" t="s">
         <v>19</v>
       </c>
-      <c r="G21" t="s">
-        <v>70</v>
+      <c r="G21">
+        <v>18.8</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -2309,25 +2342,25 @@
         <v>19</v>
       </c>
       <c r="G22">
-        <v>15.15</v>
+        <v>18.7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
@@ -2336,25 +2369,25 @@
         <v>19</v>
       </c>
       <c r="G23">
-        <v>14.9</v>
+        <v>17.7</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
         <v>77</v>
       </c>
-      <c r="B24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
-      </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -2363,52 +2396,52 @@
         <v>19</v>
       </c>
       <c r="G24">
-        <v>14.79</v>
+        <v>17.04</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
         <v>81</v>
       </c>
-      <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25">
-        <v>14.63</v>
-      </c>
       <c r="H25" s="1" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
         <v>83</v>
       </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2417,52 +2450,52 @@
         <v>19</v>
       </c>
       <c r="G26">
-        <v>11.65</v>
+        <v>15.15</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27">
+        <v>14.9</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27">
-        <v>10.26</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -2471,12 +2504,12 @@
         <v>19</v>
       </c>
       <c r="G28">
-        <v>9.21</v>
+        <v>14.79</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J28" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
@@ -2492,31 +2525,31 @@
         <v>92</v>
       </c>
       <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29">
+        <v>14.63</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29">
-        <v>8.8</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
@@ -2525,467 +2558,579 @@
         <v>19</v>
       </c>
       <c r="G30">
-        <v>8.7</v>
+        <v>11.65</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31">
+        <v>10.26</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32">
+        <v>9.21</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
         <v>100</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C33" t="s">
         <v>102</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>103</v>
       </c>
-      <c r="E31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31">
-        <v>8.22</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33">
+        <v>8.8</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B32" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32">
-        <v>8.12</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I32" s="6"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G33">
-        <v>7.81</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J33" s="6"/>
+      <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34">
+        <v>8.7</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35">
+        <v>8.22</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" t="s">
-        <v>93</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34">
-        <v>7.69</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G35">
-        <v>5.8</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J35" s="6"/>
+      <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>127</v>
+        <v>104</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
       </c>
       <c r="G36">
-        <v>5.4</v>
+        <v>8.12</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
         <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E37" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G37">
-        <v>5.4</v>
+        <v>7.81</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I37" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
-      </c>
-      <c r="F38" t="s">
-        <v>19</v>
+        <v>104</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="G38">
-        <v>5.26</v>
+        <v>7.69</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" t="s">
         <v>134</v>
       </c>
-      <c r="B39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G39">
+        <v>5.8</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E39" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G39">
-        <v>5.03</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G40">
-        <v>3.77</v>
+        <v>5.4</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B41" t="s">
+      <c r="G41">
+        <v>5.4</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C41" t="s">
-        <v>145</v>
-      </c>
-      <c r="D41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41">
-        <v>3.33</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="E42" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F42" t="s">
         <v>19</v>
       </c>
       <c r="G42">
-        <v>2.42</v>
+        <v>5.26</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G43">
-        <v>2.42</v>
+        <v>5.03</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44">
+        <v>3.77</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" t="s">
         <v>156</v>
       </c>
-      <c r="B44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>157</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E44" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="G45">
+        <v>3.33</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
         <v>159</v>
       </c>
-      <c r="G44">
+      <c r="B46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46">
         <v>2.42</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I44" s="6"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>161</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="H46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
         <v>162</v>
       </c>
-      <c r="C45" t="s">
+      <c r="B47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47">
+        <v>2.42</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D45" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" t="s">
+        <v>169</v>
+      </c>
+      <c r="E48" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48">
+        <v>2.42</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" t="s">
         <v>164</v>
       </c>
-      <c r="G45">
+      <c r="D49" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49">
         <v>1.88</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>165</v>
-      </c>
-      <c r="B46" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" t="s">
-        <v>166</v>
-      </c>
-      <c r="D46" t="s">
-        <v>167</v>
-      </c>
-      <c r="E46" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46">
+      <c r="H49" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50">
         <v>1.11</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>125</v>
+      <c r="H50" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C31" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C35" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
     <hyperlink ref="C2" r:id="rId2" display="https://seed-tars.com/1.5"/>
     <hyperlink ref="C3" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C9" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
+    <hyperlink ref="C10" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
     <hyperlink ref="F2" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
-    <hyperlink ref="F11" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
-    <hyperlink ref="F33" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
-    <hyperlink ref="F37" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
+    <hyperlink ref="F13" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
+    <hyperlink ref="F37" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
+    <hyperlink ref="F41" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
     <hyperlink ref="F6" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F36" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
-    <hyperlink ref="F44" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
-    <hyperlink ref="F35" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
-    <hyperlink ref="F34" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
-    <hyperlink ref="F40" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
-    <hyperlink ref="F39" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
-    <hyperlink ref="F41" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
-    <hyperlink ref="F43" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
-    <hyperlink ref="F45" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
+    <hyperlink ref="F40" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
+    <hyperlink ref="F48" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
+    <hyperlink ref="F39" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
+    <hyperlink ref="F38" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
+    <hyperlink ref="F44" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
+    <hyperlink ref="F43" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
+    <hyperlink ref="F45" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
+    <hyperlink ref="F47" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
+    <hyperlink ref="F49" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
     <hyperlink ref="F3" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F8" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F9" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
     <hyperlink ref="C5" r:id="rId18" display="https://github.com/bin123apple/InfantAgent"/>
     <hyperlink ref="F5" r:id="rId19" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
+    <hyperlink ref="C8" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C12" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C14" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C17" r:id="rId20" display="https://osworld-grounding.github.io/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3034,19 +3179,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -3055,21 +3200,21 @@
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -3081,102 +3226,102 @@
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -3185,128 +3330,128 @@
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3315,111 +3460,111 @@
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="D16" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3485,16 +3630,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -3506,12 +3651,12 @@
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3520,10 +3665,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3532,12 +3677,12 @@
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -3546,10 +3691,10 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -3558,47 +3703,47 @@
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -3610,21 +3755,21 @@
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -3636,76 +3781,76 @@
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -3714,50 +3859,50 @@
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3766,76 +3911,76 @@
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -3844,102 +3989,102 @@
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -3948,7 +4093,7 @@
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4010,16 +4155,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="C2" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -4031,76 +4176,76 @@
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -4109,50 +4254,50 @@
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -4161,128 +4306,128 @@
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -4291,7 +4436,7 @@
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with revised performance metrics for enhanced analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13260"/>
+    <workbookView windowWidth="27660" windowHeight="13160"/>
   </bookViews>
   <sheets>
     <sheet name="Screenshot" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="259">
   <si>
     <t>Model</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>UI-TARS-1.5 7B (100 steps)</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link</t>
   </si>
   <si>
     <t>Claude 3.7 Sonnet (50 steps)</t>
@@ -1747,7 +1750,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1873,13 +1876,13 @@
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G5">
@@ -1951,7 +1954,7 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D8" t="s">
@@ -2014,8 +2017,8 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="F10" t="s">
-        <v>19</v>
+      <c r="F10" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="G10">
         <v>26.92</v>
@@ -2027,7 +2030,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -2045,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>41</v>
@@ -2054,19 +2057,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -2081,46 +2084,46 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G13">
         <v>24.6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
@@ -2135,16 +2138,16 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -2156,22 +2159,22 @@
         <v>22.7</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -2183,25 +2186,25 @@
         <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -2216,7 +2219,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
@@ -2234,7 +2237,7 @@
         <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>41</v>
@@ -2243,7 +2246,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -2270,7 +2273,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -2288,7 +2291,7 @@
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>41</v>
@@ -2297,16 +2300,16 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -2318,22 +2321,22 @@
         <v>18.8</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -2345,22 +2348,22 @@
         <v>18.7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
@@ -2372,22 +2375,22 @@
         <v>17.7</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -2399,13 +2402,13 @@
         <v>17.04</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
@@ -2423,7 +2426,7 @@
         <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>41</v>
@@ -2432,16 +2435,16 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2453,22 +2456,22 @@
         <v>15.15</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
@@ -2480,22 +2483,22 @@
         <v>14.9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -2507,22 +2510,22 @@
         <v>14.79</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
@@ -2534,22 +2537,22 @@
         <v>14.63</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
@@ -2561,22 +2564,22 @@
         <v>11.65</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
@@ -2588,22 +2591,22 @@
         <v>10.26</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
@@ -2615,25 +2618,25 @@
         <v>9.21</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
         <v>19</v>
@@ -2642,22 +2645,22 @@
         <v>8.8</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -2669,22 +2672,22 @@
         <v>8.7</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -2696,25 +2699,25 @@
         <v>8.22</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -2723,160 +2726,160 @@
         <v>8.12</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G37">
         <v>7.81</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G38">
         <v>7.69</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G39">
         <v>5.8</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G40">
         <v>5.4</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G41">
         <v>5.4</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F42" t="s">
         <v>19</v>
@@ -2885,106 +2888,106 @@
         <v>5.26</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G43">
         <v>5.03</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
         <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G44">
         <v>3.77</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D45" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G45">
         <v>3.33</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F46" t="s">
         <v>19</v>
@@ -2993,105 +2996,105 @@
         <v>2.42</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G47">
         <v>2.42</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G48">
         <v>2.42</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D49" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G49">
         <v>1.88</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F50" t="s">
         <v>19</v>
@@ -3100,7 +3103,7 @@
         <v>1.11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3131,6 +3134,7 @@
     <hyperlink ref="C12" r:id="rId20" display="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C14" r:id="rId20" display="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C17" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="F10" r:id="rId21" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3179,19 +3183,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -3200,21 +3204,21 @@
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -3226,102 +3230,102 @@
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -3330,128 +3334,128 @@
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3460,111 +3464,111 @@
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3630,16 +3634,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -3651,12 +3655,12 @@
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -3665,10 +3669,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3677,12 +3681,12 @@
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -3691,10 +3695,10 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -3703,47 +3707,47 @@
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -3755,21 +3759,21 @@
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -3781,76 +3785,76 @@
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -3859,50 +3863,50 @@
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3911,76 +3915,76 @@
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -3989,102 +3993,102 @@
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -4093,7 +4097,7 @@
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4155,16 +4159,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -4176,76 +4180,76 @@
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -4254,50 +4258,50 @@
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -4306,128 +4310,128 @@
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -4436,7 +4440,7 @@
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with updated performance metrics for improved analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13160"/>
+    <workbookView windowWidth="27660" windowHeight="13280"/>
   </bookViews>
   <sheets>
     <sheet name="Screenshot" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="262">
   <si>
     <t>Model</t>
   </si>
@@ -56,6 +56,24 @@
     <t>Date</t>
   </si>
   <si>
+    <t>OpenAI CUA o3 (200 steps)</t>
+  </si>
+  <si>
+    <t>OpenAI</t>
+  </si>
+  <si>
+    <t>https://help.openai.com/en/articles/10561834-operator-release-notes</t>
+  </si>
+  <si>
+    <t>OpenAI, '25</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>May 23, 2025</t>
+  </si>
+  <si>
     <t>UI-TARS-1.5 (100 steps)</t>
   </si>
   <si>
@@ -89,27 +107,18 @@
     <t>Simular Research, '25</t>
   </si>
   <si>
-    <t>—</t>
-  </si>
-  <si>
     <t>https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link</t>
   </si>
   <si>
     <t>Apr 18, 2025</t>
   </si>
   <si>
-    <t>OpenAI CUA (200 steps)</t>
-  </si>
-  <si>
-    <t>OpenAI</t>
+    <t>OpenAI CUA 4o (200 steps)</t>
   </si>
   <si>
     <t>https://openai.com/index/computer-using-agent/</t>
   </si>
   <si>
-    <t>OpenAI, '25</t>
-  </si>
-  <si>
     <t>Jan 24, 2025</t>
   </si>
   <si>
@@ -245,7 +254,7 @@
     <t>~ 21</t>
   </si>
   <si>
-    <t>OpenAI CUA (15 steps)</t>
+    <t>OpenAI CUA 4o (15 steps)</t>
   </si>
   <si>
     <t>Claude 3.5 Sonnet (new) (50 steps)</t>
@@ -1425,8 +1434,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1747,10 +1756,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1796,7 +1805,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
@@ -1805,64 +1814,63 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>42.9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
         <v>42.5</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3">
-        <v>41.4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
       <c r="G4">
-        <v>38.1</v>
+        <v>41.4</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -1874,46 +1882,46 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>38.1</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5">
-        <v>35.27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G6">
-        <v>34.5</v>
+        <v>35.27</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>35</v>
@@ -1925,1078 +1933,1078 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>34.5</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="H8" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8">
-        <v>27.04</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
       <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>27</v>
+        <v>27.04</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="G10">
-        <v>26.92</v>
+        <v>27</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s">
-        <v>52</v>
+        <v>12</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11">
+        <v>26.92</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12">
-        <v>25.02</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>58</v>
+      <c r="F13" t="s">
+        <v>12</v>
       </c>
       <c r="G13">
-        <v>24.6</v>
+        <v>25.02</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
       <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
       <c r="G14">
-        <v>22.74</v>
+        <v>24.6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G15">
-        <v>22.7</v>
+        <v>22.74</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G16">
-        <v>22</v>
+        <v>22.7</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G17">
-        <v>21.8</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" t="s">
-        <v>70</v>
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>21.8</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19">
-        <v>19.7</v>
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>73</v>
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <v>19.7</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21">
-        <v>18.8</v>
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>76</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G22">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G23">
-        <v>17.7</v>
+        <v>18.7</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G24">
-        <v>17.04</v>
+        <v>17.7</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <v>17.04</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
         <v>85</v>
       </c>
-      <c r="D26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26">
-        <v>15.15</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
         <v>88</v>
       </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G27">
-        <v>14.9</v>
+        <v>15.15</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G28">
-        <v>14.79</v>
+        <v>14.9</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G29">
-        <v>14.63</v>
+        <v>14.79</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
         <v>95</v>
       </c>
-      <c r="B30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" t="s">
-        <v>92</v>
-      </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G30">
-        <v>11.65</v>
+        <v>14.63</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" t="s">
         <v>96</v>
       </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" t="s">
-        <v>79</v>
-      </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G31">
+        <v>11.65</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
         <v>10.26</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" t="s">
+      <c r="H32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>9.21</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32">
-        <v>9.21</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" t="s">
-        <v>105</v>
-      </c>
-      <c r="F33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33">
-        <v>8.8</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" t="s">
         <v>107</v>
       </c>
-      <c r="B34" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34">
+        <v>8.8</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D34" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34">
-        <v>8.7</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" t="s">
         <v>112</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>8.7</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D35" t="s">
-        <v>115</v>
-      </c>
-      <c r="E35" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35">
-        <v>8.22</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>118</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>8.22</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D36" t="s">
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
         <v>120</v>
       </c>
-      <c r="E36" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36">
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37">
         <v>8.12</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="H37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
         <v>124</v>
       </c>
-      <c r="E37" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="B38" t="s">
         <v>125</v>
       </c>
-      <c r="G37">
+      <c r="C38" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38">
         <v>7.81</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="H38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E38" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
         <v>130</v>
       </c>
-      <c r="G38">
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G39">
         <v>7.69</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I38" s="6"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="H39" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D39" t="s">
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
         <v>135</v>
       </c>
-      <c r="E39" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="B40" t="s">
         <v>136</v>
       </c>
-      <c r="G39">
-        <v>5.8</v>
-      </c>
-      <c r="H39" s="1" t="s">
+      <c r="C40" t="s">
         <v>137</v>
       </c>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
+      <c r="D40" t="s">
         <v>138</v>
       </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" t="s">
-        <v>129</v>
-      </c>
       <c r="E40" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>139</v>
       </c>
       <c r="G40">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>141</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D41" t="s">
-        <v>143</v>
-      </c>
-      <c r="E41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="G41">
         <v>5.4</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
-      </c>
-      <c r="F42" t="s">
-        <v>19</v>
+        <v>108</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="G42">
-        <v>5.26</v>
+        <v>5.4</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D43" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>149</v>
+        <v>108</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
       </c>
       <c r="G43">
-        <v>5.03</v>
+        <v>5.26</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
+        <v>149</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
         <v>151</v>
       </c>
-      <c r="B44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D44" t="s">
-        <v>148</v>
-      </c>
-      <c r="E44" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44">
+        <v>5.03</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="G44">
-        <v>3.77</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
         <v>155</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C45" t="s">
+      <c r="G45">
+        <v>3.77</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D45" t="s">
-        <v>158</v>
-      </c>
-      <c r="E45" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G45">
-        <v>3.33</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" t="s">
         <v>160</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>161</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D46" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46" t="s">
-        <v>19</v>
-      </c>
       <c r="G46">
-        <v>2.42</v>
+        <v>3.33</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="I46" s="6"/>
     </row>
@@ -3011,130 +3019,158 @@
         <v>165</v>
       </c>
       <c r="D47" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>167</v>
+        <v>108</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
       </c>
       <c r="G47">
         <v>2.42</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" t="s">
         <v>168</v>
       </c>
-      <c r="B48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>169</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>108</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="E48" t="s">
-        <v>105</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="G48">
         <v>2.42</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="6"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" t="s">
+      <c r="D49" t="s">
         <v>173</v>
       </c>
-      <c r="B49" t="s">
+      <c r="E49" t="s">
+        <v>108</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C49" t="s">
-        <v>165</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="G49">
+        <v>2.42</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E49" t="s">
-        <v>105</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G49">
-        <v>1.88</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" t="s">
         <v>177</v>
       </c>
-      <c r="B50" t="s">
-        <v>118</v>
-      </c>
       <c r="C50" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" t="s">
         <v>178</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
+        <v>108</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E50" t="s">
-        <v>105</v>
-      </c>
-      <c r="F50" t="s">
-        <v>19</v>
-      </c>
       <c r="G50">
+        <v>1.88</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" t="s">
+        <v>182</v>
+      </c>
+      <c r="E51" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51">
         <v>1.11</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>137</v>
+      <c r="H51" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://seed-tars.com/1.5"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C10" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
-    <hyperlink ref="F2" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
-    <hyperlink ref="F13" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
-    <hyperlink ref="F37" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
-    <hyperlink ref="F41" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
-    <hyperlink ref="F6" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F40" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
-    <hyperlink ref="F48" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
-    <hyperlink ref="F39" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
-    <hyperlink ref="F38" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
-    <hyperlink ref="F44" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
-    <hyperlink ref="F43" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
-    <hyperlink ref="F45" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
-    <hyperlink ref="F47" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
-    <hyperlink ref="F49" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
-    <hyperlink ref="F3" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F9" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="C5" r:id="rId18" display="https://github.com/bin123apple/InfantAgent"/>
-    <hyperlink ref="F5" r:id="rId19" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
-    <hyperlink ref="C8" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C12" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C14" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C17" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="F10" r:id="rId21" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
+    <hyperlink ref="C36" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://seed-tars.com/1.5"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
+    <hyperlink ref="C11" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
+    <hyperlink ref="F3" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
+    <hyperlink ref="F14" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
+    <hyperlink ref="F38" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
+    <hyperlink ref="F42" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
+    <hyperlink ref="F7" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F41" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
+    <hyperlink ref="F49" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
+    <hyperlink ref="F40" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
+    <hyperlink ref="F39" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
+    <hyperlink ref="F45" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
+    <hyperlink ref="F44" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
+    <hyperlink ref="F46" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
+    <hyperlink ref="F48" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
+    <hyperlink ref="F50" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
+    <hyperlink ref="F4" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F10" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="C6" r:id="rId18" display="https://github.com/bin123apple/InfantAgent"/>
+    <hyperlink ref="F6" r:id="rId19" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
+    <hyperlink ref="C9" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C13" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C15" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C18" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="F11" r:id="rId21" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
+    <hyperlink ref="C2" r:id="rId22" display="https://help.openai.com/en/articles/10561834-operator-release-notes"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3183,392 +3219,392 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" t="s">
-        <v>148</v>
-      </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -3634,470 +3670,470 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" t="s">
         <v>151</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D13" t="s">
-        <v>148</v>
-      </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G15">
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4159,288 +4195,288 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" t="s">
-        <v>148</v>
-      </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with revised performance metrics for improved analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="276">
   <si>
     <t>Model</t>
   </si>
@@ -149,6 +149,21 @@
     <t>Mar 13, 2025</t>
   </si>
   <si>
+    <t>UI-TARS-7B-1.5 + ARPO (w. gold reward)</t>
+  </si>
+  <si>
+    <t>CUHK, SmartMore, HKUST</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2505.16282</t>
+  </si>
+  <si>
+    <t>Lu, '25</t>
+  </si>
+  <si>
+    <t>Mar 22, 2025</t>
+  </si>
+  <si>
     <t>Claude 3.7 Sonnet (100 steps)</t>
   </si>
   <si>
@@ -254,6 +269,21 @@
     <t>~ 21</t>
   </si>
   <si>
+    <t>UI-TARS-7B-DPO + ZeroGUI</t>
+  </si>
+  <si>
+    <t>Shanghai AI Lab</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2505.23762</t>
+  </si>
+  <si>
+    <t>Yang et al., '25</t>
+  </si>
+  <si>
+    <t>May 30, 2025</t>
+  </si>
+  <si>
     <t>OpenAI CUA 4o (15 steps)</t>
   </si>
   <si>
@@ -327,9 +357,6 @@
   </si>
   <si>
     <t>OS-Atlas-Base-7B w/ GPT-4o</t>
-  </si>
-  <si>
-    <t>Shanghai AI Lab</t>
   </si>
   <si>
     <t>https://osatlas.github.io/</t>
@@ -1449,8 +1476,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1771,10 +1798,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1820,7 +1847,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
@@ -1977,7 +2004,7 @@
       <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D8" t="s">
@@ -1989,173 +2016,173 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>29.9</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>27.04</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
+      <c r="C10" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
       </c>
       <c r="G10">
-        <v>27</v>
+        <v>27.04</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>26.92</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>55</v>
+      <c r="F12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12">
+        <v>26.92</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="G13">
-        <v>25.02</v>
+      <c r="G13" t="s">
+        <v>60</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
       </c>
       <c r="G14">
-        <v>24.6</v>
+        <v>25.02</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I14" s="6"/>
     </row>
@@ -2164,148 +2191,148 @@
         <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="G15">
-        <v>22.74</v>
+        <v>24.6</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16">
-        <v>22.7</v>
+        <v>22.74</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>22.7</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17">
-        <v>22</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18">
-        <v>21.8</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
-        <v>73</v>
+      <c r="G19">
+        <v>21.8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -2313,26 +2340,26 @@
       <c r="F20" t="s">
         <v>12</v>
       </c>
-      <c r="G20">
-        <v>19.7</v>
+      <c r="G20" t="s">
+        <v>78</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
+        <v>80</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -2340,26 +2367,26 @@
       <c r="F21" t="s">
         <v>12</v>
       </c>
-      <c r="G21" t="s">
-        <v>76</v>
+      <c r="G21">
+        <v>20.2</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -2368,25 +2395,25 @@
         <v>12</v>
       </c>
       <c r="G22">
-        <v>18.8</v>
+        <v>19.7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -2394,26 +2421,26 @@
       <c r="F23" t="s">
         <v>12</v>
       </c>
-      <c r="G23">
-        <v>18.7</v>
+      <c r="G23" t="s">
+        <v>86</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -2422,25 +2449,25 @@
         <v>12</v>
       </c>
       <c r="G24">
-        <v>17.7</v>
+        <v>18.8</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -2449,25 +2476,25 @@
         <v>12</v>
       </c>
       <c r="G25">
-        <v>17.04</v>
+        <v>18.7</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -2475,26 +2502,26 @@
       <c r="F26" t="s">
         <v>12</v>
       </c>
-      <c r="G26" t="s">
-        <v>85</v>
+      <c r="G26">
+        <v>17.7</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -2503,25 +2530,25 @@
         <v>12</v>
       </c>
       <c r="G27">
-        <v>15.15</v>
+        <v>17.04</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>93</v>
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -2529,11 +2556,11 @@
       <c r="F28" t="s">
         <v>12</v>
       </c>
-      <c r="G28">
-        <v>14.9</v>
+      <c r="G28" t="s">
+        <v>95</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="I28" s="6"/>
     </row>
@@ -2542,13 +2569,13 @@
         <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2557,25 +2584,25 @@
         <v>12</v>
       </c>
       <c r="G29">
-        <v>14.9</v>
+        <v>15.15</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
+        <v>102</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2584,25 +2611,25 @@
         <v>12</v>
       </c>
       <c r="G30">
-        <v>14.79</v>
+        <v>14.9</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2611,25 +2638,25 @@
         <v>12</v>
       </c>
       <c r="G31">
-        <v>14.63</v>
+        <v>14.9</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2638,25 +2665,25 @@
         <v>12</v>
       </c>
       <c r="G32">
-        <v>11.65</v>
+        <v>14.79</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2665,25 +2692,25 @@
         <v>12</v>
       </c>
       <c r="G33">
-        <v>10.26</v>
+        <v>14.63</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2692,154 +2719,154 @@
         <v>12</v>
       </c>
       <c r="G34">
-        <v>9.21</v>
+        <v>11.65</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J34" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>10.26</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>9.21</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" t="s">
-        <v>113</v>
-      </c>
-      <c r="F35" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35">
-        <v>8.8</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I35" s="6"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36">
-        <v>8.7</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
         <v>120</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37">
+        <v>8.8</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37">
-        <v>8.22</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
         <v>125</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>126</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>127</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38">
+        <v>8.7</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E38" t="s">
-        <v>113</v>
-      </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38">
-        <v>8.12</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>129</v>
       </c>
       <c r="B39" t="s">
         <v>130</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>131</v>
       </c>
       <c r="D39" t="s">
         <v>132</v>
       </c>
       <c r="E39" t="s">
-        <v>113</v>
-      </c>
-      <c r="F39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39">
+        <v>8.22</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G39">
-        <v>7.81</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J39" s="6"/>
+      <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" t="s">
         <v>135</v>
-      </c>
-      <c r="B40" t="s">
-        <v>9</v>
       </c>
       <c r="C40" t="s">
         <v>136</v>
@@ -2848,178 +2875,178 @@
         <v>137</v>
       </c>
       <c r="E40" t="s">
-        <v>113</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>138</v>
+        <v>122</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
       </c>
       <c r="G40">
-        <v>7.69</v>
+        <v>8.12</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" t="s">
         <v>140</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>141</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D41" t="s">
+      <c r="G41">
+        <v>7.81</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E41" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G41">
-        <v>5.8</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>147</v>
       </c>
       <c r="G42">
-        <v>5.4</v>
+        <v>7.69</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>148</v>
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>149</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E43" t="s">
-        <v>113</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>152</v>
+        <v>122</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="G43">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I43" s="6"/>
+        <v>154</v>
+      </c>
+      <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E44" t="s">
-        <v>113</v>
-      </c>
-      <c r="F44" t="s">
-        <v>12</v>
+        <v>122</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="G44">
-        <v>5.26</v>
+        <v>5.4</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D45" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E45" t="s">
-        <v>113</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>157</v>
+        <v>122</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="G45">
-        <v>5.03</v>
+        <v>5.4</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D46" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
-        <v>113</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>161</v>
+        <v>122</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
       </c>
       <c r="G46">
-        <v>3.77</v>
+        <v>5.26</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I46" s="6"/>
     </row>
@@ -3028,25 +3055,25 @@
         <v>163</v>
       </c>
       <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
         <v>164</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>165</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E47" t="s">
-        <v>113</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47">
+        <v>5.03</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="G47">
-        <v>3.33</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="I47" s="6"/>
     </row>
@@ -3055,114 +3082,115 @@
         <v>168</v>
       </c>
       <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
         <v>169</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D48" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" t="s">
-        <v>113</v>
-      </c>
-      <c r="F48" t="s">
-        <v>12</v>
-      </c>
       <c r="G48">
-        <v>2.42</v>
+        <v>3.77</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G49">
+        <v>3.33</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B49" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" t="s">
-        <v>173</v>
-      </c>
-      <c r="D49" t="s">
-        <v>174</v>
-      </c>
-      <c r="E49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G49">
-        <v>2.42</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>178</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D50" t="s">
-        <v>178</v>
+        <v>73</v>
       </c>
       <c r="E50" t="s">
-        <v>113</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>179</v>
+        <v>122</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
       </c>
       <c r="G50">
         <v>2.42</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
         <v>180</v>
       </c>
-      <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>181</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>182</v>
-      </c>
-      <c r="C51" t="s">
-        <v>173</v>
       </c>
       <c r="D51" t="s">
         <v>183</v>
       </c>
       <c r="E51" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>184</v>
       </c>
       <c r="G51">
-        <v>1.88</v>
+        <v>2.42</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>171</v>
+      </c>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>185</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C52" t="s">
         <v>186</v>
@@ -3171,49 +3199,104 @@
         <v>187</v>
       </c>
       <c r="E52" t="s">
-        <v>113</v>
-      </c>
-      <c r="F52" t="s">
-        <v>12</v>
+        <v>122</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="G52">
+        <v>2.42</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" t="s">
+        <v>192</v>
+      </c>
+      <c r="E53" t="s">
+        <v>122</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G53">
+        <v>1.88</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>194</v>
+      </c>
+      <c r="B54" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" t="s">
+        <v>195</v>
+      </c>
+      <c r="D54" t="s">
+        <v>196</v>
+      </c>
+      <c r="E54" t="s">
+        <v>122</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54">
         <v>1.11</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>145</v>
+      <c r="H54" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C37" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C39" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
     <hyperlink ref="C3" r:id="rId2" display="https://seed-tars.com/1.5"/>
     <hyperlink ref="C4" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C11" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
+    <hyperlink ref="C12" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
     <hyperlink ref="F3" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
-    <hyperlink ref="F14" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
-    <hyperlink ref="F39" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
-    <hyperlink ref="F43" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
+    <hyperlink ref="F15" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
+    <hyperlink ref="F41" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
+    <hyperlink ref="F45" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
     <hyperlink ref="F7" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F42" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
-    <hyperlink ref="F50" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
-    <hyperlink ref="F41" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
-    <hyperlink ref="F40" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
-    <hyperlink ref="F46" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
-    <hyperlink ref="F45" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
-    <hyperlink ref="F47" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
-    <hyperlink ref="F49" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
-    <hyperlink ref="F51" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
+    <hyperlink ref="F44" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
+    <hyperlink ref="F52" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
+    <hyperlink ref="F43" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
+    <hyperlink ref="F42" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
+    <hyperlink ref="F48" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
+    <hyperlink ref="F47" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
+    <hyperlink ref="F49" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
+    <hyperlink ref="F51" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
+    <hyperlink ref="F53" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
     <hyperlink ref="F4" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F10" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F11" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
     <hyperlink ref="C6" r:id="rId18" display="https://github.com/bin123apple/InfantAgent"/>
     <hyperlink ref="F6" r:id="rId19" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
-    <hyperlink ref="C9" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C13" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C15" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C18" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="F11" r:id="rId21" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
+    <hyperlink ref="C10" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C14" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C16" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C19" r:id="rId20" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="F12" r:id="rId21" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
     <hyperlink ref="C2" r:id="rId22" display="https://help.openai.com/en/articles/10561834-operator-release-notes"/>
-    <hyperlink ref="C28" r:id="rId23" display="https://arxiv.org/abs/2505.13909"/>
+    <hyperlink ref="C30" r:id="rId23" display="https://arxiv.org/abs/2505.13909"/>
+    <hyperlink ref="C8" r:id="rId24" display="https://arxiv.org/abs/2505.16282"/>
+    <hyperlink ref="C21" r:id="rId25" display="https://arxiv.org/abs/2505.23762"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3262,19 +3345,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -3283,21 +3366,21 @@
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -3309,102 +3392,102 @@
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -3413,128 +3496,128 @@
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C12" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D12" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -3543,111 +3626,111 @@
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D13" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3713,16 +3796,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -3734,12 +3817,12 @@
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -3748,10 +3831,10 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -3760,12 +3843,12 @@
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -3774,10 +3857,10 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -3786,47 +3869,47 @@
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
         <v>239</v>
       </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>230</v>
-      </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -3838,21 +3921,21 @@
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" t="s">
         <v>240</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" t="s">
-        <v>231</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -3864,76 +3947,76 @@
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -3942,50 +4025,50 @@
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="D12" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -3994,76 +4077,76 @@
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -4072,102 +4155,102 @@
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -4176,7 +4259,7 @@
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4202,7 +4285,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -4238,16 +4321,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -4259,76 +4342,76 @@
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -4337,50 +4420,50 @@
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -4389,128 +4472,128 @@
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -4519,7 +4602,7 @@
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with further revised performance metrics for improved analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="277">
   <si>
     <t>Model</t>
   </si>
@@ -128,7 +128,10 @@
     <t>Evolution intelligence &amp; University of Minnesota</t>
   </si>
   <si>
-    <t>https://github.com/bin123apple/InfantAgent</t>
+    <t>https://arxiv.org/abs/2505.10887</t>
+  </si>
+  <si>
+    <t>Lei et al., '25</t>
   </si>
   <si>
     <t>Planner: Claude-3.7 Sonnet，Grounder: UI-TARS-1.5-7B</t>
@@ -1801,7 +1804,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1956,29 +1959,32 @@
       <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="G6">
         <v>35.27</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -1993,22 +1999,22 @@
         <v>34.5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -2020,22 +2026,22 @@
         <v>29.9</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -2044,28 +2050,28 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -2074,19 +2080,19 @@
         <v>27.04</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -2101,13 +2107,13 @@
         <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -2122,7 +2128,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12">
         <v>26.92</v>
@@ -2134,16 +2140,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -2152,28 +2158,28 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -2182,52 +2188,52 @@
         <v>25.02</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15">
         <v>24.6</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -2236,22 +2242,22 @@
         <v>22.74</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -2263,22 +2269,22 @@
         <v>22.7</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -2290,25 +2296,25 @@
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -2317,22 +2323,22 @@
         <v>21.8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -2341,25 +2347,25 @@
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -2371,13 +2377,13 @@
         <v>20.2</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -2404,16 +2410,16 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -2422,25 +2428,25 @@
         <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -2452,22 +2458,22 @@
         <v>18.8</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -2479,22 +2485,22 @@
         <v>18.7</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -2506,22 +2512,22 @@
         <v>17.7</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -2533,22 +2539,22 @@
         <v>17.04</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -2557,25 +2563,25 @@
         <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2587,22 +2593,22 @@
         <v>15.15</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2614,22 +2620,22 @@
         <v>14.9</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2641,22 +2647,22 @@
         <v>14.9</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2668,22 +2674,22 @@
         <v>14.79</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2695,22 +2701,22 @@
         <v>14.63</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2722,22 +2728,22 @@
         <v>11.65</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2749,22 +2755,22 @@
         <v>10.26</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -2776,25 +2782,25 @@
         <v>9.21</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -2803,22 +2809,22 @@
         <v>8.8</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2830,22 +2836,22 @@
         <v>8.7</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2857,25 +2863,25 @@
         <v>8.22</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -2884,160 +2890,160 @@
         <v>8.12</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G41">
         <v>7.81</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G42">
         <v>7.69</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E43" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G43">
         <v>5.8</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G44">
         <v>5.4</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D45" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E45" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G45">
         <v>5.4</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -3046,106 +3052,106 @@
         <v>5.26</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G47">
         <v>5.03</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G48">
         <v>3.77</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G49">
         <v>3.33</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B50" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C50" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E50" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
@@ -3154,105 +3160,105 @@
         <v>2.42</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C51" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E51" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G51">
         <v>2.42</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D52" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G52">
         <v>2.42</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B53" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D53" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E53" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G53">
         <v>1.88</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C54" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D54" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E54" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
@@ -3261,7 +3267,7 @@
         <v>1.11</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3286,17 +3292,17 @@
     <hyperlink ref="F53" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
     <hyperlink ref="F4" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
     <hyperlink ref="F11" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="C6" r:id="rId18" display="https://github.com/bin123apple/InfantAgent"/>
-    <hyperlink ref="F6" r:id="rId19" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
-    <hyperlink ref="C10" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C14" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C16" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C19" r:id="rId20" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="F12" r:id="rId21" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
-    <hyperlink ref="C2" r:id="rId22" display="https://help.openai.com/en/articles/10561834-operator-release-notes"/>
-    <hyperlink ref="C30" r:id="rId23" display="https://arxiv.org/abs/2505.13909"/>
-    <hyperlink ref="C8" r:id="rId24" display="https://arxiv.org/abs/2505.16282"/>
-    <hyperlink ref="C21" r:id="rId25" display="https://arxiv.org/abs/2505.23762"/>
+    <hyperlink ref="F6" r:id="rId18" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
+    <hyperlink ref="C10" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C14" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C16" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C19" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="F12" r:id="rId20" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
+    <hyperlink ref="C2" r:id="rId21" display="https://help.openai.com/en/articles/10561834-operator-release-notes"/>
+    <hyperlink ref="C30" r:id="rId22" display="https://arxiv.org/abs/2505.13909"/>
+    <hyperlink ref="C8" r:id="rId23" display="https://arxiv.org/abs/2505.16282"/>
+    <hyperlink ref="C21" r:id="rId24" display="https://arxiv.org/abs/2505.23762"/>
+    <hyperlink ref="C6" r:id="rId25" display="https://arxiv.org/abs/2505.10887"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3345,19 +3351,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -3366,21 +3372,21 @@
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -3392,102 +3398,102 @@
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -3496,128 +3502,128 @@
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -3626,111 +3632,111 @@
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3796,16 +3802,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -3817,24 +3823,24 @@
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -3843,24 +3849,24 @@
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -3869,47 +3875,47 @@
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -3921,21 +3927,21 @@
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -3947,76 +3953,76 @@
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -4025,50 +4031,50 @@
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -4077,76 +4083,76 @@
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -4155,102 +4161,102 @@
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -4259,7 +4265,7 @@
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4321,16 +4327,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -4342,76 +4348,76 @@
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -4420,50 +4426,50 @@
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -4472,128 +4478,128 @@
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -4602,7 +4608,7 @@
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with further updated performance metrics for enhanced analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13200"/>
+    <workbookView windowWidth="27660" windowHeight="13280"/>
   </bookViews>
   <sheets>
     <sheet name="Screenshot" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="282">
   <si>
     <t>Model</t>
   </si>
@@ -56,6 +56,24 @@
     <t>Date</t>
   </si>
   <si>
+    <t>GTA1  w/ o3 (100 steps)</t>
+  </si>
+  <si>
+    <t>Salesforce &amp; The Australian National University &amp; The University of Hong Kong</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1GvNXwDt5_U-ned49urVlOFj1FBi86ddT?usp=sharing</t>
+  </si>
+  <si>
+    <t>July 7, 2025</t>
+  </si>
+  <si>
     <t>OpenAI CUA o3 (200 steps)</t>
   </si>
   <si>
@@ -66,9 +84,6 @@
   </si>
   <si>
     <t>OpenAI, '25</t>
-  </si>
-  <si>
-    <t>—</t>
   </si>
   <si>
     <t>May 23, 2025</t>
@@ -1474,13 +1489,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1541,6 +1559,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1801,10 +1826,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1850,20 +1875,17 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>42.9</v>
+      <c r="G2" s="6">
+        <v>45.2</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
@@ -1876,159 +1898,158 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>42.9</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
         <v>42.5</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4">
-        <v>41.4</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="G5">
-        <v>38.1</v>
+        <v>41.4</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>38.1</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6">
-        <v>35.27</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>34.5</v>
+        <v>35.27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="G8">
-        <v>29.9</v>
+        <v>34.5</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -2037,565 +2058,565 @@
       <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>29.9</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>27.04</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
+      <c r="C11" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>25</v>
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>27</v>
+        <v>27.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="G12">
-        <v>26.92</v>
+        <v>27</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>61</v>
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13">
+        <v>26.92</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14">
-        <v>25.02</v>
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
       </c>
       <c r="G15">
-        <v>24.6</v>
+        <v>25.02</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I15" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="G16">
-        <v>22.74</v>
+        <v>24.6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17">
-        <v>22.7</v>
+        <v>22.74</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18">
+        <v>22.7</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18">
-        <v>22</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>21.8</v>
+        <v>22</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" t="s">
-        <v>79</v>
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <v>21.8</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21">
-        <v>20.2</v>
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>84</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I21" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
+        <v>86</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22">
-        <v>19.7</v>
+        <v>20.2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" t="s">
-        <v>87</v>
+        <v>11</v>
+      </c>
+      <c r="G23">
+        <v>19.7</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24">
-        <v>18.8</v>
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>92</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I24" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26">
-        <v>17.7</v>
+        <v>18.7</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I26" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <v>17.04</v>
+        <v>17.7</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I27" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" t="s">
-        <v>96</v>
+        <v>11</v>
+      </c>
+      <c r="G28">
+        <v>17.04</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29">
-        <v>15.15</v>
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>101</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
@@ -2604,241 +2625,241 @@
       <c r="B30" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" t="s">
         <v>104</v>
       </c>
       <c r="D30" t="s">
         <v>105</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30">
-        <v>14.9</v>
+        <v>15.15</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I30" s="6"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
+        <v>108</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31">
         <v>14.9</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I31" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32">
-        <v>14.79</v>
+        <v>14.9</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I32" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33">
-        <v>14.63</v>
+        <v>14.79</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I33" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34">
-        <v>11.65</v>
+        <v>14.63</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I34" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35">
+        <v>11.65</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36">
         <v>10.26</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I35" s="6"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="H36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>9.21</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36">
-        <v>9.21</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" t="s">
-        <v>121</v>
-      </c>
-      <c r="D37" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" t="s">
-        <v>123</v>
-      </c>
-      <c r="F37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37">
-        <v>8.8</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I37" s="6"/>
+      <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
         <v>125</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>126</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>127</v>
       </c>
-      <c r="D38" t="s">
-        <v>128</v>
-      </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
@@ -2847,25 +2868,25 @@
       <c r="B39" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>132</v>
       </c>
       <c r="D39" t="s">
         <v>133</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39">
-        <v>8.22</v>
+        <v>8.7</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I39" s="6"/>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
@@ -2874,59 +2895,59 @@
       <c r="B40" t="s">
         <v>136</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D40" t="s">
         <v>138</v>
       </c>
       <c r="E40" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G40">
+        <v>8.22</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41">
         <v>8.12</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" s="6"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
-        <v>139</v>
-      </c>
-      <c r="B41" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" t="s">
-        <v>141</v>
-      </c>
-      <c r="D41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E41" t="s">
-        <v>123</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G41">
-        <v>7.81</v>
-      </c>
       <c r="H41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
         <v>144</v>
       </c>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>145</v>
-      </c>
-      <c r="B42" t="s">
-        <v>9</v>
       </c>
       <c r="C42" t="s">
         <v>146</v>
@@ -2935,90 +2956,90 @@
         <v>147</v>
       </c>
       <c r="E42" t="s">
-        <v>123</v>
-      </c>
-      <c r="F42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>148</v>
       </c>
       <c r="G42">
-        <v>7.69</v>
+        <v>7.81</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I42" s="6"/>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="J42" s="7"/>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>150</v>
       </c>
       <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
         <v>151</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>152</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
+        <v>128</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E43" t="s">
-        <v>123</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43">
+        <v>7.69</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G43">
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G44">
         <v>5.8</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" t="s">
-        <v>146</v>
-      </c>
-      <c r="D44" t="s">
-        <v>147</v>
-      </c>
-      <c r="E44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G44">
-        <v>5.4</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I44" s="6"/>
+        <v>160</v>
+      </c>
+      <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
         <v>151</v>
       </c>
-      <c r="C45" t="s">
-        <v>160</v>
-      </c>
       <c r="D45" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E45" t="s">
-        <v>123</v>
-      </c>
-      <c r="F45" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>162</v>
       </c>
       <c r="G45">
@@ -3027,115 +3048,115 @@
       <c r="H45" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I45" s="6"/>
+      <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="E46" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" t="s">
-        <v>12</v>
+        <v>128</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="G46">
-        <v>5.26</v>
+        <v>5.4</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I46" s="6"/>
+        <v>168</v>
+      </c>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D47" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>167</v>
+        <v>128</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
       </c>
       <c r="G47">
-        <v>5.03</v>
+        <v>5.26</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I47" s="6"/>
+        <v>160</v>
+      </c>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>169</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
         <v>170</v>
       </c>
       <c r="D48" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G48">
-        <v>3.77</v>
+        <v>5.03</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I48" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
         <v>175</v>
       </c>
       <c r="D49" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E49" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49">
+        <v>3.77</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G49">
-        <v>3.33</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I49" s="6"/>
+      <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
@@ -3148,161 +3169,189 @@
         <v>180</v>
       </c>
       <c r="D50" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="E50" t="s">
-        <v>123</v>
-      </c>
-      <c r="F50" t="s">
-        <v>12</v>
+        <v>128</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="G50">
-        <v>2.42</v>
+        <v>3.33</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I50" s="6"/>
+        <v>177</v>
+      </c>
+      <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>184</v>
+        <v>79</v>
       </c>
       <c r="E51" t="s">
-        <v>123</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>185</v>
+        <v>128</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
       </c>
       <c r="G51">
         <v>2.42</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I51" s="6"/>
+        <v>160</v>
+      </c>
+      <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>186</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E52" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G52">
         <v>2.42</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="1:8">
+        <v>177</v>
+      </c>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>191</v>
       </c>
       <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
         <v>192</v>
-      </c>
-      <c r="C53" t="s">
-        <v>183</v>
       </c>
       <c r="D53" t="s">
         <v>193</v>
       </c>
       <c r="E53" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>194</v>
       </c>
       <c r="G53">
-        <v>1.88</v>
+        <v>2.42</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>172</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="I53" s="7"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D54" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E54" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" t="s">
-        <v>12</v>
+        <v>128</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="G54">
+        <v>1.88</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55">
         <v>1.11</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>155</v>
+      <c r="H55" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C39" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://seed-tars.com/1.5"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C12" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
-    <hyperlink ref="F3" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
-    <hyperlink ref="F15" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
-    <hyperlink ref="F41" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
-    <hyperlink ref="F45" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
-    <hyperlink ref="F7" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F44" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
-    <hyperlink ref="F52" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
-    <hyperlink ref="F43" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
-    <hyperlink ref="F42" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
-    <hyperlink ref="F48" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
-    <hyperlink ref="F47" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
-    <hyperlink ref="F49" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
-    <hyperlink ref="F51" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
-    <hyperlink ref="F53" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
-    <hyperlink ref="F4" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F11" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
-    <hyperlink ref="F6" r:id="rId18" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
-    <hyperlink ref="C10" r:id="rId19" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C14" r:id="rId19" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C16" r:id="rId19" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C19" r:id="rId19" display="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="F12" r:id="rId20" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
-    <hyperlink ref="C2" r:id="rId21" display="https://help.openai.com/en/articles/10561834-operator-release-notes"/>
-    <hyperlink ref="C30" r:id="rId22" display="https://arxiv.org/abs/2505.13909"/>
-    <hyperlink ref="C8" r:id="rId23" display="https://arxiv.org/abs/2505.16282"/>
-    <hyperlink ref="C21" r:id="rId24" display="https://arxiv.org/abs/2505.23762"/>
-    <hyperlink ref="C6" r:id="rId25" display="https://arxiv.org/abs/2505.10887"/>
+    <hyperlink ref="C40" r:id="rId1" display="https://arxiv.org/abs/2504.07491"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://seed-tars.com/1.5"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://github.com/simular-ai/Agent-S"/>
+    <hyperlink ref="C13" r:id="rId2" display="https://seed-tars.com/1.5" tooltip="https://seed-tars.com/1.5"/>
+    <hyperlink ref="F4" r:id="rId4" display="https://drive.google.com/file/d/1e7SCYqpxFX2FCGEOhf6jcVvwkx3leIKf/view?usp=drive_link"/>
+    <hyperlink ref="F16" r:id="rId5" display="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link" tooltip="https://drive.google.com/file/d/1vUWlXVenkOc5F1s-z8DdpfU4Y5fUMssr/view?usp=drive_link"/>
+    <hyperlink ref="F42" r:id="rId6" display="https://drive.google.com/drive/folders/14_xlL-e0-0INq2O1THbhFKi6Z0bgfwR4?usp=drive_link"/>
+    <hyperlink ref="F46" r:id="rId7" display="https://drive.google.com/drive/folders/1j-YVzEGAGWxXgse75MCnhUCTVuejM76A?usp=drive_link"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link" tooltip="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F45" r:id="rId9" display="https://drive.google.com/drive/folders/1NLsHdLUNZOHsEC5xNZ4e4PHkDC5IELjj?usp=drive_link"/>
+    <hyperlink ref="F53" r:id="rId10" display="https://drive.google.com/drive/folders/1iBOXZpknCi1Fqzg0fQMG6CZc9NWrwdkf?usp=drive_link"/>
+    <hyperlink ref="F44" r:id="rId11" display="https://drive.google.com/file/d/17jgZEjslxIZPC5kuzOq6oTK5EuDiJ-_l/view?usp=drive_link"/>
+    <hyperlink ref="F43" r:id="rId12" display="https://drive.google.com/file/d/1miMp-AR_hOfLUWszGb_aZG2f_Nd66Ntt/view?usp=drive_link"/>
+    <hyperlink ref="F49" r:id="rId13" display="https://drive.google.com/file/d/1Skq_uMcAR08LMDnIpOswjxm5ntbVXm5M/view?usp=drive_link"/>
+    <hyperlink ref="F48" r:id="rId14" display="https://drive.google.com/file/d/1mN12zjCiawfU4k1ifPsLW-hcuzPV7Voz/view?usp=drive_link"/>
+    <hyperlink ref="F50" r:id="rId15" display="https://drive.google.com/file/d/1KSYs7ZOhEkjBQX5UnMpLkbxZZ6BLhbDm/view?usp=drive_link"/>
+    <hyperlink ref="F52" r:id="rId16" display="https://drive.google.com/file/d/1geppLqwV80p66bXdffVBbLayjCkIQ9mk/view?usp=drive_link"/>
+    <hyperlink ref="F54" r:id="rId17" display="https://drive.google.com/file/d/1T58G_EIr4pWZYJ8plXEWspFHr35g-Nsy/view?usp=drive_link"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F12" r:id="rId8" display="https://drive.google.com/drive/folders/18PTnMwgyhxIWTVNLMwf0sbzhvh9AlVqE?usp=drive_link"/>
+    <hyperlink ref="F7" r:id="rId18" display="https://drive.google.com/file/d/1M-PAz9S7cvYR8T6-VIEZKMbw7yVTN5je/view?usp=drive_link"/>
+    <hyperlink ref="C11" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C15" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C17" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C20" r:id="rId19" display="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="F13" r:id="rId20" display="https://drive.google.com/file/d/1t-w6OAQHfmRplHbi93aWXZlOBwOQkwY2/view?usp=drive_link"/>
+    <hyperlink ref="C3" r:id="rId21" display="https://help.openai.com/en/articles/10561834-operator-release-notes"/>
+    <hyperlink ref="C31" r:id="rId22" display="https://arxiv.org/abs/2505.13909"/>
+    <hyperlink ref="C9" r:id="rId23" display="https://arxiv.org/abs/2505.16282"/>
+    <hyperlink ref="C22" r:id="rId24" display="https://arxiv.org/abs/2505.23762"/>
+    <hyperlink ref="C7" r:id="rId25" display="https://arxiv.org/abs/2505.10887"/>
+    <hyperlink ref="F2" r:id="rId26" display="https://drive.google.com/drive/folders/1GvNXwDt5_U-ned49urVlOFj1FBi86ddT?usp=sharing"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -3351,392 +3400,392 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>22.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>16.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G4">
         <v>12.24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="G5">
         <v>11.36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="G6">
         <v>10.82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E7" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>10.3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G8">
         <v>6.87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="G9">
         <v>6.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="G10">
         <v>4.81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G11">
         <v>4.32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>2.98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G13">
         <v>2.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="G14">
         <v>2.69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="G15">
         <v>2.37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C16" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="G16">
         <v>1.61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3802,470 +3851,470 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>23.85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>20.58</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>20.48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="G5">
         <v>19.39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D6" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>17.34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>13.55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G8">
         <v>12.17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="G9">
         <v>11.21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>11.11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G11">
         <v>9.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D12" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>8.94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="G13">
         <v>6.21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G14">
         <v>5.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>4.41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="G17">
         <v>3.48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="G18">
         <v>2.42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19">
         <v>1.32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4327,288 +4376,288 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>24.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="G3">
         <v>11.77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="G4">
         <v>8.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>7.79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="G6">
         <v>6.72</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>5.4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="G8">
         <v>4.59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="G10">
         <v>2.42</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="G11">
         <v>1.06</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>0.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark_data.xlsx with further refined performance metrics for enhanced analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/benchmark_data.xlsx
+++ b/static/data/benchmark_data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="282">
   <si>
     <t>Model</t>
   </si>
@@ -65,6 +65,9 @@
     <t>TBD</t>
   </si>
   <si>
+    <t>Yang et al., '25</t>
+  </si>
+  <si>
     <t>—</t>
   </si>
   <si>
@@ -294,9 +297,6 @@
   </si>
   <si>
     <t>https://arxiv.org/abs/2505.23762</t>
-  </si>
-  <si>
-    <t>Yang et al., '25</t>
   </si>
   <si>
     <t>May 30, 2025</t>
@@ -1829,7 +1829,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1878,548 +1878,551 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6">
         <v>45.2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>42.9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>42.5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>41.4</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>38.1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>35.27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>34.5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <v>29.9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <v>27.04</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12">
         <v>27</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G13">
         <v>26.92</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15">
         <v>25.02</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G16">
         <v>24.6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17">
         <v>22.74</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>22.7</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>22</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20">
         <v>21.8</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22">
         <v>20.2</v>
@@ -2434,25 +2437,25 @@
         <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23">
         <v>19.7</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I23" s="7"/>
     </row>
@@ -2461,25 +2464,25 @@
         <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
         <v>92</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I24" s="7"/>
     </row>
@@ -2488,25 +2491,25 @@
         <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25">
         <v>18.8</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I25" s="7"/>
     </row>
@@ -2515,25 +2518,25 @@
         <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26">
         <v>18.7</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I26" s="7"/>
     </row>
@@ -2542,25 +2545,25 @@
         <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27">
         <v>17.7</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I27" s="7"/>
     </row>
@@ -2569,7 +2572,7 @@
         <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>97</v>
@@ -2578,10 +2581,10 @@
         <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28">
         <v>17.04</v>
@@ -2596,25 +2599,25 @@
         <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
         <v>101</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I29" s="7"/>
     </row>
@@ -2632,10 +2635,10 @@
         <v>105</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G30">
         <v>15.15</v>
@@ -2659,10 +2662,10 @@
         <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G31">
         <v>14.9</v>
@@ -2677,25 +2680,25 @@
         <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G32">
         <v>14.9</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I32" s="7"/>
     </row>
@@ -2704,7 +2707,7 @@
         <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>97</v>
@@ -2713,10 +2716,10 @@
         <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33">
         <v>14.79</v>
@@ -2731,7 +2734,7 @@
         <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
         <v>115</v>
@@ -2740,10 +2743,10 @@
         <v>116</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34">
         <v>14.63</v>
@@ -2758,7 +2761,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
         <v>115</v>
@@ -2767,10 +2770,10 @@
         <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G35">
         <v>11.65</v>
@@ -2785,7 +2788,7 @@
         <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
         <v>97</v>
@@ -2794,10 +2797,10 @@
         <v>98</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36">
         <v>10.26</v>
@@ -2821,10 +2824,10 @@
         <v>123</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37">
         <v>9.21</v>
@@ -2851,7 +2854,7 @@
         <v>128</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38">
         <v>8.8</v>
@@ -2875,10 +2878,10 @@
         <v>133</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39">
         <v>8.7</v>
@@ -2902,10 +2905,10 @@
         <v>138</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40">
         <v>8.22</v>
@@ -2932,7 +2935,7 @@
         <v>128</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41">
         <v>8.12</v>
@@ -2974,7 +2977,7 @@
         <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
         <v>151</v>
@@ -3028,7 +3031,7 @@
         <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
         <v>151</v>
@@ -3082,7 +3085,7 @@
         <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
         <v>151</v>
@@ -3094,7 +3097,7 @@
         <v>128</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G47">
         <v>5.26</v>
@@ -3109,7 +3112,7 @@
         <v>169</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
         <v>170</v>
@@ -3136,7 +3139,7 @@
         <v>174</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>175</v>
@@ -3196,13 +3199,13 @@
         <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
         <v>128</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51">
         <v>2.42</v>
@@ -3309,7 +3312,7 @@
         <v>128</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G55">
         <v>1.11</v>
@@ -3415,7 +3418,7 @@
         <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>22.5</v>
@@ -3438,10 +3441,10 @@
         <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>16.6</v>
@@ -3455,7 +3458,7 @@
         <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>215</v>
@@ -3481,7 +3484,7 @@
         <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>170</v>
@@ -3507,7 +3510,7 @@
         <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>151</v>
@@ -3545,7 +3548,7 @@
         <v>207</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>10.3</v>
@@ -3585,7 +3588,7 @@
         <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>175</v>
@@ -3675,7 +3678,7 @@
         <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>2.98</v>
@@ -3715,7 +3718,7 @@
         <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>234</v>
@@ -3854,7 +3857,7 @@
         <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>245</v>
@@ -3863,10 +3866,10 @@
         <v>246</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>23.85</v>
@@ -3880,10 +3883,10 @@
         <v>248</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>249</v>
@@ -3892,7 +3895,7 @@
         <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>20.58</v>
@@ -3906,10 +3909,10 @@
         <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
         <v>249</v>
@@ -3918,7 +3921,7 @@
         <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>20.48</v>
@@ -3941,7 +3944,7 @@
         <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>252</v>
@@ -3958,7 +3961,7 @@
         <v>254</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>245</v>
@@ -3967,10 +3970,10 @@
         <v>246</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>17.34</v>
@@ -3984,7 +3987,7 @@
         <v>255</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>245</v>
@@ -3993,10 +3996,10 @@
         <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>13.55</v>
@@ -4010,7 +4013,7 @@
         <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>151</v>
@@ -4036,7 +4039,7 @@
         <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>170</v>
@@ -4062,7 +4065,7 @@
         <v>258</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>259</v>
@@ -4074,7 +4077,7 @@
         <v>128</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>11.11</v>
@@ -4088,7 +4091,7 @@
         <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>151</v>
@@ -4126,7 +4129,7 @@
         <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>8.94</v>
@@ -4140,7 +4143,7 @@
         <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>175</v>
@@ -4198,13 +4201,13 @@
         <v>185</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
         <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15">
         <v>4.41</v>
@@ -4308,7 +4311,7 @@
         <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>1.32</v>
@@ -4388,10 +4391,10 @@
         <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>24.5</v>
@@ -4405,7 +4408,7 @@
         <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>151</v>
@@ -4431,7 +4434,7 @@
         <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -4469,7 +4472,7 @@
         <v>128</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>7.79</v>
@@ -4489,7 +4492,7 @@
         <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>128</v>
@@ -4521,7 +4524,7 @@
         <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>5.4</v>
@@ -4535,7 +4538,7 @@
         <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>170</v>
@@ -4561,7 +4564,7 @@
         <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>175</v>
@@ -4651,7 +4654,7 @@
         <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>0.99</v>

</xml_diff>